<commit_message>
add duplicate links and not www handling
</commit_message>
<xml_diff>
--- a/windows_executable/Links.xlsx
+++ b/windows_executable/Links.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1515" yWindow="1515" windowWidth="23175" windowHeight="13695" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20940" yWindow="2295" windowWidth="15645" windowHeight="12735" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Links" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -77,11 +77,26 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
       <sz val="18"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
     </font>
     <font/>
     <font>
@@ -260,7 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
@@ -289,11 +304,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -301,16 +319,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -340,19 +358,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -360,7 +379,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -453,20 +472,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
@@ -476,7 +486,7 @@
         <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -807,38 +817,38 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H54"/>
+  <dimension ref="B2:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.875" defaultRowHeight="15.75" outlineLevelCol="0"/>
   <cols>
-    <col width="10.875" customWidth="1" style="22" min="1" max="1"/>
-    <col width="15" customWidth="1" style="22" min="2" max="2"/>
-    <col width="62.875" customWidth="1" style="22" min="3" max="3"/>
-    <col width="16" customWidth="1" style="22" min="4" max="4"/>
-    <col width="18.375" customWidth="1" style="22" min="5" max="5"/>
-    <col width="23.125" customWidth="1" style="22" min="6" max="6"/>
-    <col width="32.125" customWidth="1" style="22" min="7" max="7"/>
-    <col width="46.625" customWidth="1" style="22" min="8" max="8"/>
-    <col width="10.875" customWidth="1" style="22" min="9" max="70"/>
-    <col width="10.875" customWidth="1" style="22" min="71" max="16384"/>
+    <col width="10.875" customWidth="1" style="23" min="1" max="1"/>
+    <col width="17" customWidth="1" style="23" min="2" max="2"/>
+    <col width="62.875" customWidth="1" style="23" min="3" max="3"/>
+    <col width="16" customWidth="1" style="23" min="4" max="4"/>
+    <col width="18.375" customWidth="1" style="23" min="5" max="5"/>
+    <col width="23.125" customWidth="1" style="23" min="6" max="6"/>
+    <col width="32.125" customWidth="1" style="23" min="7" max="7"/>
+    <col width="46.625" customWidth="1" style="23" min="8" max="8"/>
+    <col width="10.875" customWidth="1" style="23" min="9" max="76"/>
+    <col width="10.875" customWidth="1" style="23" min="77" max="16384"/>
   </cols>
   <sheetData>
     <row r="2" ht="45" customHeight="1">
-      <c r="B2" s="31" t="inlineStr">
+      <c r="B2" s="32" t="inlineStr">
         <is>
           <t>TABELA DE OBTENÇÃO DE DADOS</t>
         </is>
       </c>
-      <c r="C2" s="28" t="n"/>
-      <c r="D2" s="28" t="n"/>
-      <c r="E2" s="28" t="n"/>
-      <c r="F2" s="28" t="n"/>
-      <c r="G2" s="28" t="n"/>
-      <c r="H2" s="29" t="n"/>
+      <c r="C2" s="29" t="n"/>
+      <c r="D2" s="29" t="n"/>
+      <c r="E2" s="29" t="n"/>
+      <c r="F2" s="29" t="n"/>
+      <c r="G2" s="29" t="n"/>
+      <c r="H2" s="30" t="n"/>
     </row>
     <row r="3" ht="26.1" customHeight="1">
       <c r="B3" s="6" t="n"/>
@@ -849,68 +859,67 @@
       <c r="H3" s="5" t="n"/>
     </row>
     <row r="4" ht="29.1" customHeight="1">
-      <c r="B4" s="27" t="inlineStr">
+      <c r="B4" s="28" t="inlineStr">
         <is>
           <t>Configurações:</t>
         </is>
       </c>
-      <c r="C4" s="28" t="n"/>
-      <c r="D4" s="29" t="n"/>
-      <c r="F4" s="27" t="inlineStr">
+      <c r="C4" s="29" t="n"/>
+      <c r="D4" s="30" t="n"/>
+      <c r="F4" s="28" t="inlineStr">
         <is>
           <t>Instruções:</t>
         </is>
       </c>
-      <c r="G4" s="28" t="n"/>
-      <c r="H4" s="29" t="n"/>
-    </row>
-    <row r="5" ht="48.75" customHeight="1">
-      <c r="B5" s="30" t="inlineStr">
+      <c r="G4" s="29" t="n"/>
+      <c r="H4" s="30" t="n"/>
+    </row>
+    <row r="5" ht="36.95" customHeight="1">
+      <c r="B5" s="31" t="inlineStr">
         <is>
           <t>Apenas obter dados dos links cujos campos da linha estão vazios (mais seguro)</t>
         </is>
       </c>
-      <c r="C5" s="20" t="n"/>
-      <c r="D5" s="11" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F5" s="18" t="inlineStr">
+      <c r="C5" s="21" t="n"/>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F5" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">    1. Insira o novo link na primeira linha vazia da tabela, na coluna de "Links".
     2. Não se preocupe nem com o estilo, nem com os valores das células da nova linha. Tudo isso será arrumado pelo programa.
-    3. Salve e feche o Excel.
-    4. Execute o programa "webcrawler.exe".</t>
-        </is>
-      </c>
-      <c r="G5" s="19" t="n"/>
-      <c r="H5" s="20" t="n"/>
+    3. Vá para a linha de comando na pasta deste arquivo e execute "scrapy crawl linkedin". Caso haja erros, siga as instruções que aparecerem na tela.</t>
+        </is>
+      </c>
+      <c r="G5" s="20" t="n"/>
+      <c r="H5" s="21" t="n"/>
     </row>
     <row r="6" ht="45.95" customHeight="1">
-      <c r="B6" s="32" t="inlineStr">
-        <is>
-          <t>Tentar obter dados de páginas que foram marcadas como "Não é uma pessoa" (ligue apenas se achar que há erros)</t>
-        </is>
-      </c>
-      <c r="C6" s="29" t="n"/>
-      <c r="D6" s="31" t="inlineStr">
+      <c r="B6" s="33" t="inlineStr">
+        <is>
+          <t>Tentar obter dados de páginas que foram marcadas como "Não é uma pessoa"</t>
+        </is>
+      </c>
+      <c r="C6" s="30" t="n"/>
+      <c r="D6" s="32" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="E6" s="10" t="n"/>
-      <c r="F6" s="21" t="n"/>
-      <c r="H6" s="23" t="n"/>
+      <c r="E6" s="12" t="n"/>
+      <c r="F6" s="22" t="n"/>
+      <c r="H6" s="24" t="n"/>
     </row>
     <row r="7" ht="39" customHeight="1">
-      <c r="D7" s="10" t="n"/>
-      <c r="E7" s="10" t="n"/>
-      <c r="F7" s="24" t="n"/>
-      <c r="G7" s="25" t="n"/>
-      <c r="H7" s="26" t="n"/>
-    </row>
-    <row r="9" ht="20.1" customHeight="1">
+      <c r="D7" s="12" t="n"/>
+      <c r="E7" s="12" t="n"/>
+      <c r="F7" s="25" t="n"/>
+      <c r="G7" s="26" t="n"/>
+      <c r="H7" s="27" t="n"/>
+    </row>
+    <row r="9" ht="18.75" customHeight="1">
       <c r="B9" s="8" t="inlineStr">
         <is>
           <t>Conta existe</t>
@@ -947,38 +956,38 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="339.95" customHeight="1">
-      <c r="B10" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C10" s="36" t="inlineStr">
+    <row r="10" ht="315" customHeight="1">
+      <c r="B10" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C10" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/rebecca-liu-93a12a28/</t>
         </is>
       </c>
-      <c r="D10" s="36" t="inlineStr">
+      <c r="D10" s="38" t="inlineStr">
         <is>
           <t>Rebecca</t>
         </is>
       </c>
-      <c r="E10" s="36" t="inlineStr">
+      <c r="E10" s="38" t="inlineStr">
         <is>
           <t>Liu</t>
         </is>
       </c>
-      <c r="F10" s="36" t="inlineStr">
+      <c r="F10" s="38" t="inlineStr">
         <is>
           <t>Senior Consultant at The Talent Company Ltd.</t>
         </is>
       </c>
-      <c r="G10" s="36" t="inlineStr">
-        <is>
-          <t>Toronto e Região, Canadá</t>
-        </is>
-      </c>
-      <c r="H10" s="36" t="inlineStr">
+      <c r="G10" s="38" t="inlineStr">
+        <is>
+          <t>Toronto, Canada Area</t>
+        </is>
+      </c>
+      <c r="H10" s="38" t="inlineStr">
         <is>
           <t>The Talent Company is an HR Solutions Firm. We work closely with our clients to FIND, KEEP, REWARD and TRANSITION their talent. 
 With offices in Toronto, Mississauga and Markham, we support our clients in building, developing and retaining a highly engaged, high-performing workforce that is focused on achieving their business strategies and goals.
@@ -992,349 +1001,369 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="33.95" customHeight="1">
-      <c r="B11" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C11" s="34" t="inlineStr">
+    <row r="11" ht="31.5" customHeight="1">
+      <c r="B11" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C11" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/ed-woodward-7ba2b968</t>
         </is>
       </c>
-      <c r="D11" s="36" t="inlineStr">
+      <c r="D11" s="38" t="inlineStr">
         <is>
           <t>Ed</t>
         </is>
       </c>
-      <c r="E11" s="36" t="inlineStr">
+      <c r="E11" s="38" t="inlineStr">
         <is>
           <t>Woodward</t>
         </is>
       </c>
-      <c r="F11" s="36" t="inlineStr">
+      <c r="F11" s="38" t="inlineStr">
         <is>
           <t>General Manager at Northstar CG, LP.</t>
         </is>
       </c>
-      <c r="G11" s="36" t="inlineStr">
+      <c r="G11" s="38" t="inlineStr">
         <is>
           <t>La Center, Washington</t>
         </is>
       </c>
-      <c r="H11" s="36" t="inlineStr">
+      <c r="H11" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="135.95" customHeight="1">
-      <c r="B12" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C12" s="34" t="inlineStr">
+    <row r="12" ht="126" customHeight="1">
+      <c r="B12" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C12" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/neil-bath-76621045</t>
         </is>
       </c>
-      <c r="D12" s="36" t="inlineStr">
+      <c r="D12" s="38" t="inlineStr">
         <is>
           <t>Neil</t>
         </is>
       </c>
-      <c r="E12" s="36" t="inlineStr">
+      <c r="E12" s="38" t="inlineStr">
         <is>
           <t>Bath</t>
         </is>
       </c>
-      <c r="F12" s="36" t="inlineStr">
+      <c r="F12" s="38" t="inlineStr">
         <is>
           <t>Marine insurance broker</t>
         </is>
       </c>
-      <c r="G12" s="36" t="inlineStr">
+      <c r="G12" s="38" t="inlineStr">
         <is>
           <t>Miami, Florida</t>
         </is>
       </c>
-      <c r="H12" s="36" t="inlineStr">
+      <c r="H12" s="38" t="inlineStr">
         <is>
           <t>Many years of experience in all aspects of Marine Insurance &amp; Reinsurance, including business development, client servicing, placing of business and handling of claims. Specializing primarily in Hull &amp; Machinery, Protection &amp; Indemnity, Charterers Liabilities, Port &amp; Terminal Operators, Marine Cargo including STP's, with particular emphasis on Latin America.</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="170.1" customHeight="1">
-      <c r="B13" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C13" s="34" t="inlineStr">
+    <row r="13" ht="157.5" customHeight="1">
+      <c r="B13" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C13" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jim-cassell-171918b8</t>
         </is>
       </c>
-      <c r="D13" s="36" t="inlineStr">
+      <c r="D13" s="38" t="inlineStr">
         <is>
           <t>Jim</t>
         </is>
       </c>
-      <c r="E13" s="36" t="inlineStr">
+      <c r="E13" s="38" t="inlineStr">
         <is>
           <t>Cassell</t>
         </is>
       </c>
-      <c r="F13" s="36" t="inlineStr">
+      <c r="F13" s="38" t="inlineStr">
         <is>
           <t>GIS Engineering Technician at NiSource</t>
         </is>
       </c>
-      <c r="G13" s="36" t="inlineStr">
-        <is>
-          <t>Columbus, Ohio e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H13" s="36" t="inlineStr">
+      <c r="G13" s="38" t="inlineStr">
+        <is>
+          <t>Columbus, Ohio Area</t>
+        </is>
+      </c>
+      <c r="H13" s="38" t="inlineStr">
         <is>
           <t>As a professional in the field of business applications who also has a background in customer service, I have unique insight into both sides of business processes.  I have experience in determining requirements for process improvement projects, as well as testing and training during project implementation.  I also have extensive experience in the system administration side of applications support.  This experience has given me a big picture perspective on business processes.</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="24.95" customHeight="1">
-      <c r="B14" s="35" t="inlineStr">
-        <is>
-          <t>Não é uma pessoa</t>
-        </is>
-      </c>
-      <c r="C14" s="34" t="inlineStr">
+    <row r="14" ht="23.25" customHeight="1">
+      <c r="B14" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C14" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/claudio-silveira-888b741b0/</t>
         </is>
       </c>
-      <c r="D14" s="36" t="n"/>
-      <c r="E14" s="36" t="n"/>
-      <c r="F14" s="36" t="n"/>
-      <c r="G14" s="36" t="n"/>
-      <c r="H14" s="36" t="n"/>
-    </row>
-    <row r="15" ht="170.1" customHeight="1">
-      <c r="B15" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C15" s="34" t="inlineStr">
+      <c r="D14" s="38" t="inlineStr">
+        <is>
+          <t>Claudio</t>
+        </is>
+      </c>
+      <c r="E14" s="38" t="inlineStr">
+        <is>
+          <t>Silveira</t>
+        </is>
+      </c>
+      <c r="F14" s="38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G14" s="38" t="inlineStr">
+        <is>
+          <t>Brazil</t>
+        </is>
+      </c>
+      <c r="H14" s="38" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="157.5" customHeight="1">
+      <c r="B15" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C15" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/boristai?trk=public_profile_browsemap_profile-result-card_result-card_full-click</t>
         </is>
       </c>
-      <c r="D15" s="36" t="inlineStr">
+      <c r="D15" s="38" t="inlineStr">
         <is>
           <t>Boris</t>
         </is>
       </c>
-      <c r="E15" s="36" t="inlineStr">
+      <c r="E15" s="38" t="inlineStr">
         <is>
           <t>Tai</t>
         </is>
       </c>
-      <c r="F15" s="36" t="inlineStr">
+      <c r="F15" s="38" t="inlineStr">
         <is>
           <t>Talent Acquisition Specialist at Loblaw Data Insight &amp; Analytics</t>
         </is>
       </c>
-      <c r="G15" s="36" t="inlineStr">
-        <is>
-          <t>Toronto e Região, Canadá</t>
-        </is>
-      </c>
-      <c r="H15" s="36" t="inlineStr">
+      <c r="G15" s="38" t="inlineStr">
+        <is>
+          <t>Toronto, Canada Area</t>
+        </is>
+      </c>
+      <c r="H15" s="38" t="inlineStr">
         <is>
           <t>Experienced as a recruitment consultant providing recruiting services to banking and financial clients in the GTA area. Specializing in IT and business roles for both contract and full time positions. It is my goal to provide a smooth recruitment process for client and candidates, ensuring that the best possible talent is delivered in a quick and efficient manner.
 Specialties: Recruitment, Client Management, Human Resources</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="51" customHeight="1">
-      <c r="B16" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C16" s="34" t="inlineStr">
+    <row r="16" ht="47.25" customHeight="1">
+      <c r="B16" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C16" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/sammar-badawi?trk=public_profile_browsemap_profile-result-card_result-card_full-click</t>
         </is>
       </c>
-      <c r="D16" s="36" t="inlineStr">
+      <c r="D16" s="38" t="inlineStr">
         <is>
           <t>Sammar</t>
         </is>
       </c>
-      <c r="E16" s="36" t="inlineStr">
+      <c r="E16" s="38" t="inlineStr">
         <is>
           <t>Badawi</t>
         </is>
       </c>
-      <c r="F16" s="36" t="inlineStr">
+      <c r="F16" s="38" t="inlineStr">
         <is>
           <t>Talent Acquisition Partner at FreshBooks - We're Hiring!</t>
         </is>
       </c>
-      <c r="G16" s="36" t="inlineStr">
-        <is>
-          <t>Toronto, Ontario, Canadá</t>
-        </is>
-      </c>
-      <c r="H16" s="36" t="inlineStr">
+      <c r="G16" s="38" t="inlineStr">
+        <is>
+          <t>Toronto, Ontario, Canada</t>
+        </is>
+      </c>
+      <c r="H16" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="51" customHeight="1">
-      <c r="B17" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C17" s="34" t="inlineStr">
+    <row r="17" ht="47.25" customHeight="1">
+      <c r="B17" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C17" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jessica-portelini-a09972161?trk=public_profile_browsemap_profile-result-card_result-card_full-click</t>
         </is>
       </c>
-      <c r="D17" s="36" t="inlineStr">
+      <c r="D17" s="38" t="inlineStr">
         <is>
           <t>Jessica</t>
         </is>
       </c>
-      <c r="E17" s="36" t="inlineStr">
+      <c r="E17" s="38" t="inlineStr">
         <is>
           <t>Portelini</t>
         </is>
       </c>
-      <c r="F17" s="36" t="inlineStr">
+      <c r="F17" s="38" t="inlineStr">
         <is>
           <t>Recruitment Manager at Apex Talent - We're Hiring Now!</t>
         </is>
       </c>
-      <c r="G17" s="36" t="inlineStr">
-        <is>
-          <t>Toronto e Região, Canadá</t>
-        </is>
-      </c>
-      <c r="H17" s="36" t="inlineStr">
+      <c r="G17" s="38" t="inlineStr">
+        <is>
+          <t>Toronto, Canada Area</t>
+        </is>
+      </c>
+      <c r="H17" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="50.1" customHeight="1">
-      <c r="B18" s="35" t="inlineStr">
+    <row r="18" ht="46.5" customHeight="1">
+      <c r="B18" s="37" t="inlineStr">
         <is>
           <t>Não é uma pessoa</t>
         </is>
       </c>
-      <c r="C18" s="34" t="inlineStr">
+      <c r="C18" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jim-cassell-171918b7</t>
         </is>
       </c>
-      <c r="D18" s="36" t="n"/>
-      <c r="E18" s="36" t="n"/>
-      <c r="F18" s="36" t="n"/>
-      <c r="G18" s="36" t="n"/>
-      <c r="H18" s="36" t="n"/>
-    </row>
-    <row r="19" ht="50.1" customHeight="1">
-      <c r="B19" s="35" t="inlineStr">
+      <c r="D18" s="38" t="n"/>
+      <c r="E18" s="38" t="n"/>
+      <c r="F18" s="38" t="n"/>
+      <c r="G18" s="38" t="n"/>
+      <c r="H18" s="38" t="n"/>
+    </row>
+    <row r="19" ht="46.5" customHeight="1">
+      <c r="B19" s="37" t="inlineStr">
         <is>
           <t>Não é uma pessoa</t>
         </is>
       </c>
-      <c r="C19" s="34" t="inlineStr">
+      <c r="C19" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/mark/</t>
         </is>
       </c>
-      <c r="D19" s="36" t="n"/>
-      <c r="E19" s="36" t="n"/>
-      <c r="F19" s="36" t="n"/>
-      <c r="G19" s="36" t="n"/>
-      <c r="H19" s="36" t="n"/>
-    </row>
-    <row r="20" ht="153" customHeight="1">
-      <c r="B20" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C20" s="34" t="inlineStr">
+      <c r="D19" s="38" t="n"/>
+      <c r="E19" s="38" t="n"/>
+      <c r="F19" s="38" t="n"/>
+      <c r="G19" s="38" t="n"/>
+      <c r="H19" s="38" t="n"/>
+    </row>
+    <row r="20" ht="141.75" customHeight="1">
+      <c r="B20" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C20" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/kaelahrussell/</t>
         </is>
       </c>
-      <c r="D20" s="36" t="inlineStr">
+      <c r="D20" s="38" t="inlineStr">
         <is>
           <t>Kaelah</t>
         </is>
       </c>
-      <c r="E20" s="36" t="inlineStr">
+      <c r="E20" s="38" t="inlineStr">
         <is>
           <t>Russell</t>
         </is>
       </c>
-      <c r="F20" s="36" t="inlineStr">
+      <c r="F20" s="38" t="inlineStr">
         <is>
           <t>Senior Talent Acquisition Partner at Prodigy Game</t>
         </is>
       </c>
-      <c r="G20" s="36" t="inlineStr">
-        <is>
-          <t>Toronto, Ontario, Canadá</t>
-        </is>
-      </c>
-      <c r="H20" s="36" t="inlineStr">
+      <c r="G20" s="38" t="inlineStr">
+        <is>
+          <t>Toronto, Ontario, Canada</t>
+        </is>
+      </c>
+      <c r="H20" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">We've all heard that saying 'do what you love, and love what you do'. Well, I'm happy to say that's exactly what I'm doing!  I've built a career in talent acquisition, starting in the agency world, then transitioned to corporate recruitment. I've become a trusted business partner and advisor when it comes to all things recruitment.  I love the excitement in finding the right person and helping Prodigy Game become stronger and better by adding top talent. </t>
         </is>
       </c>
     </row>
-    <row r="21" ht="204" customHeight="1">
-      <c r="B21" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C21" s="36" t="inlineStr">
+    <row r="21" ht="189" customHeight="1">
+      <c r="B21" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C21" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/bencrenca</t>
         </is>
       </c>
-      <c r="D21" s="36" t="inlineStr">
+      <c r="D21" s="38" t="inlineStr">
         <is>
           <t>Ben</t>
         </is>
       </c>
-      <c r="E21" s="36" t="inlineStr">
+      <c r="E21" s="38" t="inlineStr">
         <is>
           <t>Crenca</t>
         </is>
       </c>
-      <c r="F21" s="36" t="inlineStr">
+      <c r="F21" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Talent Acquisition | Employer Branding | Building Culture </t>
         </is>
       </c>
-      <c r="G21" s="36" t="inlineStr">
-        <is>
-          <t>Washington D.C. Metro e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H21" s="36" t="inlineStr">
+      <c r="G21" s="38" t="inlineStr">
+        <is>
+          <t>Washington D.C. Metro Area</t>
+        </is>
+      </c>
+      <c r="H21" s="38" t="inlineStr">
         <is>
           <t>WE ARE HIRING!
 Currently Seeking: 
@@ -1345,37 +1374,37 @@
       </c>
     </row>
     <row r="22" ht="409.5" customHeight="1">
-      <c r="B22" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C22" s="36" t="inlineStr">
+      <c r="B22" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C22" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/mandyj</t>
         </is>
       </c>
-      <c r="D22" s="36" t="inlineStr">
+      <c r="D22" s="38" t="inlineStr">
         <is>
           <t>Mandy</t>
         </is>
       </c>
-      <c r="E22" s="36" t="inlineStr">
+      <c r="E22" s="38" t="inlineStr">
         <is>
           <t>Jenkins</t>
         </is>
       </c>
-      <c r="F22" s="36" t="inlineStr">
+      <c r="F22" s="38" t="inlineStr">
         <is>
           <t>General Manager, The Compass Experiment at McClatchy</t>
         </is>
       </c>
-      <c r="G22" s="36" t="inlineStr">
-        <is>
-          <t>Nova Iorque, Nova Iorque</t>
-        </is>
-      </c>
-      <c r="H22" s="36" t="inlineStr">
+      <c r="G22" s="38" t="inlineStr">
+        <is>
+          <t>New York, New York</t>
+        </is>
+      </c>
+      <c r="H22" s="38" t="inlineStr">
         <is>
           <t>I started in digital journalism at a time when most jobs didn’t yet have titles, there were just tasks to be done and few people with the skills to do them. Now, after more than 16 years of working in newsrooms spanning newspapers, radio, television, service providers and digital startups, I am currently taking time out of the industry to be a fellow in the 2018-19 fellowship class of the John S. Knight fellowship at Stanford, where I will focus my research on disinformation and user experience. I am also currently the president of the Online News Association, the world's largest organization for digital journalists and media innovators. 
 I was most recently the Editor in Chief at Storyful, the leading social news and insights agency. I managed a team of 60+ social journalists who worked with the world's top newsrooms in surfacing, verifying and acquiring eyewitness journalism and debunking disinformation.  
@@ -1385,37 +1414,37 @@
       </c>
     </row>
     <row r="23" ht="409.5" customHeight="1">
-      <c r="B23" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C23" s="36" t="inlineStr">
+      <c r="B23" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C23" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/neilkane</t>
         </is>
       </c>
-      <c r="D23" s="36" t="inlineStr">
+      <c r="D23" s="38" t="inlineStr">
         <is>
           <t>Neil</t>
         </is>
       </c>
-      <c r="E23" s="36" t="inlineStr">
+      <c r="E23" s="38" t="inlineStr">
         <is>
           <t>Kane</t>
         </is>
       </c>
-      <c r="F23" s="36" t="inlineStr">
+      <c r="F23" s="38" t="inlineStr">
         <is>
           <t>Executive | Entrepreneur | Educator | Startup CEO  Author "The Innovator's Secret Formula"</t>
         </is>
       </c>
-      <c r="G23" s="36" t="inlineStr">
-        <is>
-          <t>Grande Detroit e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H23" s="36" t="inlineStr">
+      <c r="G23" s="38" t="inlineStr">
+        <is>
+          <t>Greater Detroit Area</t>
+        </is>
+      </c>
+      <c r="H23" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">"I've never been qualified for any job that I've had, but I always achieved success."​
 *  Entrepreneur/executive/innovator with 25 years of general management, sales, marketing and investment experience in environments ranging from nanotechnology to advanced materials to consumer products. 
@@ -1448,112 +1477,112 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="33.95" customHeight="1">
-      <c r="B24" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C24" s="36" t="inlineStr">
+    <row r="24" ht="31.5" customHeight="1">
+      <c r="B24" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C24" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/dixonheath</t>
         </is>
       </c>
-      <c r="D24" s="36" t="inlineStr">
+      <c r="D24" s="38" t="inlineStr">
         <is>
           <t>Heath</t>
         </is>
       </c>
-      <c r="E24" s="36" t="inlineStr">
+      <c r="E24" s="38" t="inlineStr">
         <is>
           <t>Dixon</t>
         </is>
       </c>
-      <c r="F24" s="36" t="inlineStr">
+      <c r="F24" s="38" t="inlineStr">
         <is>
           <t>Technology Lawyer at Amazon</t>
         </is>
       </c>
-      <c r="G24" s="36" t="inlineStr">
-        <is>
-          <t>Grande Seattle e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H24" s="36" t="inlineStr">
+      <c r="G24" s="38" t="inlineStr">
+        <is>
+          <t>Greater Seattle Area</t>
+        </is>
+      </c>
+      <c r="H24" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Want to join the Amazon Legal Team?  Want to change the Internet?  </t>
         </is>
       </c>
     </row>
-    <row r="25" ht="204" customHeight="1">
-      <c r="B25" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C25" s="36" t="inlineStr">
+    <row r="25" ht="173.25" customHeight="1">
+      <c r="B25" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C25" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/erineriksson</t>
         </is>
       </c>
-      <c r="D25" s="36" t="inlineStr">
+      <c r="D25" s="38" t="inlineStr">
         <is>
           <t>Erin Elise</t>
         </is>
       </c>
-      <c r="E25" s="36" t="inlineStr">
+      <c r="E25" s="38" t="inlineStr">
         <is>
           <t>Eriksson</t>
         </is>
       </c>
-      <c r="F25" s="36" t="inlineStr">
+      <c r="F25" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Social Impact, Global Health, &amp; Philanthropy Consultant </t>
         </is>
       </c>
-      <c r="G25" s="36" t="inlineStr">
-        <is>
-          <t>Nova Iorque, Nova Iorque</t>
-        </is>
-      </c>
-      <c r="H25" s="36" t="inlineStr">
+      <c r="G25" s="38" t="inlineStr">
+        <is>
+          <t>New York, New York</t>
+        </is>
+      </c>
+      <c r="H25" s="38" t="inlineStr">
         <is>
           <t>Experienced CSR professional and funder working with private sector, government, foundations, nonprofits, and bilateral/multilateral funders to improve global health outcomes. Success developing new strategic initiatives and enhancing brand visibility. Experience overseeing finances, budgeting, operations, and audit process for corporate foundation. Focus on corporate citizenship/corporate social responsibility, philanthropy, HIV/AIDS, monitoring &amp; evaluation, maternal health, key populations, social drivers, and employee engagement.</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="186.95" customHeight="1">
-      <c r="B26" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C26" s="36" t="inlineStr">
+    <row r="26" ht="141.75" customHeight="1">
+      <c r="B26" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C26" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/crystalhuang89</t>
         </is>
       </c>
-      <c r="D26" s="36" t="inlineStr">
+      <c r="D26" s="38" t="inlineStr">
         <is>
           <t>Crystal</t>
         </is>
       </c>
-      <c r="E26" s="36" t="inlineStr">
+      <c r="E26" s="38" t="inlineStr">
         <is>
           <t>Huang</t>
         </is>
       </c>
-      <c r="F26" s="36" t="inlineStr">
+      <c r="F26" s="38" t="inlineStr">
         <is>
           <t>Principal at New Enterprise Associates (NEA)</t>
         </is>
       </c>
-      <c r="G26" s="36" t="inlineStr">
-        <is>
-          <t>Nova Iorque, Nova Iorque</t>
-        </is>
-      </c>
-      <c r="H26" s="36" t="inlineStr">
+      <c r="G26" s="38" t="inlineStr">
+        <is>
+          <t>New York, New York</t>
+        </is>
+      </c>
+      <c r="H26" s="38" t="inlineStr">
         <is>
           <t>Venture capitalist at New Enterprise Associates (NEA) in New York, covering enterprise technologies (SaaS, infrastructure, security) and consumer internet. 
 Previously I was at GGV Capital in Silicon Valley where I worked closely with companies including Aptible, BigCommerce, BitSight, BrightWheel, HashiCorp, Headspin, MileZero, NS1, OpenDoor, Restless Bandit, Slack, Tile, Tray.io, Unravel Data and Wish.</t>
@@ -1561,37 +1590,37 @@
       </c>
     </row>
     <row r="27" ht="409.5" customHeight="1">
-      <c r="B27" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C27" s="36" t="inlineStr">
+      <c r="B27" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C27" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jasonhengels</t>
         </is>
       </c>
-      <c r="D27" s="36" t="inlineStr">
+      <c r="D27" s="38" t="inlineStr">
         <is>
           <t>Jason</t>
         </is>
       </c>
-      <c r="E27" s="36" t="inlineStr">
+      <c r="E27" s="38" t="inlineStr">
         <is>
           <t>Hengels</t>
         </is>
       </c>
-      <c r="F27" s="36" t="inlineStr">
+      <c r="F27" s="38" t="inlineStr">
         <is>
           <t>Founder, Exposure Security</t>
         </is>
       </c>
-      <c r="G27" s="36" t="inlineStr">
+      <c r="G27" s="38" t="inlineStr">
         <is>
           <t>Redwood City, California</t>
         </is>
       </c>
-      <c r="H27" s="36" t="inlineStr">
+      <c r="H27" s="38" t="inlineStr">
         <is>
           <t>Jason Hengels is a security executive with a broad range of skills who leads by example and creates an environment of excellence. He currently provides CISO-for-hire services to high profile companies, including industry names in the payment, insurance, multimedia and mortgage verticals. 
 Jason has worked through some of the most difficult situations in the security world, including APT breaches and remediation work, extortion attempts and DDoS attacks. He has led companies through PCI, SOC 2 and other compliance efforts and has presented at large conferences such as RSA. Beginning in 2014, Jason helped develop and refine the Information Security curriculum at Merritt College. Prior to founding Exposure Security, Jason built the Information Security programs at companies such as Box and CyberSource and held a senior-level position at Visa.
@@ -1600,223 +1629,223 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="51" customHeight="1">
-      <c r="B28" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C28" s="36" t="inlineStr">
+    <row r="28" ht="47.25" customHeight="1">
+      <c r="B28" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C28" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/ginamartinez13</t>
         </is>
       </c>
-      <c r="D28" s="36" t="inlineStr">
+      <c r="D28" s="38" t="inlineStr">
         <is>
           <t>Gina</t>
         </is>
       </c>
-      <c r="E28" s="36" t="inlineStr">
+      <c r="E28" s="38" t="inlineStr">
         <is>
           <t>Martinez</t>
         </is>
       </c>
-      <c r="F28" s="36" t="inlineStr">
+      <c r="F28" s="38" t="inlineStr">
         <is>
           <t>Breaking News Reporter</t>
         </is>
       </c>
-      <c r="G28" s="36" t="inlineStr">
-        <is>
-          <t>Brooklyn, Nova Iorque</t>
-        </is>
-      </c>
-      <c r="H28" s="36" t="inlineStr">
+      <c r="G28" s="38" t="inlineStr">
+        <is>
+          <t>Brooklyn, New York</t>
+        </is>
+      </c>
+      <c r="H28" s="38" t="inlineStr">
         <is>
           <t>Experienced breaking news reporter with knowledge of social media, great interviewing skills and talent for news gathering in a busy news room.</t>
         </is>
       </c>
     </row>
-    <row r="29" ht="24.95" customHeight="1">
-      <c r="B29" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C29" s="36" t="inlineStr">
+    <row r="29" ht="23.25" customHeight="1">
+      <c r="B29" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C29" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/noobjun</t>
         </is>
       </c>
-      <c r="D29" s="36" t="inlineStr">
+      <c r="D29" s="38" t="inlineStr">
         <is>
           <t>Jun</t>
         </is>
       </c>
-      <c r="E29" s="36" t="inlineStr">
+      <c r="E29" s="38" t="inlineStr">
         <is>
           <t>Zhou</t>
         </is>
       </c>
-      <c r="F29" s="36" t="inlineStr">
+      <c r="F29" s="38" t="inlineStr">
         <is>
           <t>Software Engineer</t>
         </is>
       </c>
-      <c r="G29" s="36" t="inlineStr">
+      <c r="G29" s="38" t="inlineStr">
         <is>
           <t>Mountain View, California</t>
         </is>
       </c>
-      <c r="H29" s="36" t="inlineStr">
+      <c r="H29" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="33.95" customHeight="1">
-      <c r="B30" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C30" s="36" t="inlineStr">
+    <row r="30" ht="31.5" customHeight="1">
+      <c r="B30" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C30" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/priyabhardwaj</t>
         </is>
       </c>
-      <c r="D30" s="36" t="inlineStr">
+      <c r="D30" s="38" t="inlineStr">
         <is>
           <t>Priya</t>
         </is>
       </c>
-      <c r="E30" s="36" t="inlineStr">
+      <c r="E30" s="38" t="inlineStr">
         <is>
           <t>Bhardwaj</t>
         </is>
       </c>
-      <c r="F30" s="36" t="inlineStr">
+      <c r="F30" s="38" t="inlineStr">
         <is>
           <t>Vice President at JPMorgan Chase</t>
         </is>
       </c>
-      <c r="G30" s="36" t="inlineStr">
-        <is>
-          <t>Cidade de Nova Iorque e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H30" s="36" t="inlineStr">
+      <c r="G30" s="38" t="inlineStr">
+        <is>
+          <t>Greater New York City Area</t>
+        </is>
+      </c>
+      <c r="H30" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="31" ht="51" customHeight="1">
-      <c r="B31" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C31" s="36" t="inlineStr">
+    <row r="31" ht="47.25" customHeight="1">
+      <c r="B31" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C31" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/mattniksch</t>
         </is>
       </c>
-      <c r="D31" s="36" t="inlineStr">
+      <c r="D31" s="38" t="inlineStr">
         <is>
           <t>Matt</t>
         </is>
       </c>
-      <c r="E31" s="36" t="inlineStr">
+      <c r="E31" s="38" t="inlineStr">
         <is>
           <t>Niksch</t>
         </is>
       </c>
-      <c r="F31" s="36" t="inlineStr">
+      <c r="F31" s="38" t="inlineStr">
         <is>
           <t>President at Noble Network of Charter Schools</t>
         </is>
       </c>
-      <c r="G31" s="36" t="inlineStr">
-        <is>
-          <t>Grande Chicago e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H31" s="36" t="inlineStr">
+      <c r="G31" s="38" t="inlineStr">
+        <is>
+          <t>Greater Chicago Area</t>
+        </is>
+      </c>
+      <c r="H31" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="237.95" customHeight="1">
-      <c r="B32" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C32" s="36" t="inlineStr">
+    <row r="32" ht="204.75" customHeight="1">
+      <c r="B32" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C32" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/iw3dlyw7</t>
         </is>
       </c>
-      <c r="D32" s="36" t="inlineStr">
+      <c r="D32" s="38" t="inlineStr">
         <is>
           <t>Jason</t>
         </is>
       </c>
-      <c r="E32" s="36" t="inlineStr">
+      <c r="E32" s="38" t="inlineStr">
         <is>
           <t>Child</t>
         </is>
       </c>
-      <c r="F32" s="36" t="inlineStr">
+      <c r="F32" s="38" t="inlineStr">
         <is>
           <t>CFO at Splunk</t>
         </is>
       </c>
-      <c r="G32" s="36" t="inlineStr">
-        <is>
-          <t>Baía de São Francisco e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H32" s="36" t="inlineStr">
+      <c r="G32" s="38" t="inlineStr">
+        <is>
+          <t>San Francisco Bay Area</t>
+        </is>
+      </c>
+      <c r="H32" s="38" t="inlineStr">
         <is>
           <t>Over 28 years of progressive experience in all aspects of Finance &amp; Strategy, Accounting, Capital Markets and Treasury. Specialize in scaling disruptive companies and working with/learning/gaining insight from awesome people.  Finance Director/VP during Amazon.com's growth from $900M sales run-rate in early 1999, to $50B+ run-rate in late 2010.  CFO during Groupon's growth from $750M in sales in 2010 to $7.6B in 2014.  CFO during Opendoor's growth from $400M in run-rate sales in early 2017 to $4B in early 2019.  Now, CFO during Splunk's transformation from on-prem to Cloud/Saas, while maintaining 40%+ annualized growth on our path to $5B in Revenue.</t>
         </is>
       </c>
     </row>
     <row r="33" ht="409.5" customHeight="1">
-      <c r="B33" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C33" s="36" t="inlineStr">
+      <c r="B33" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C33" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/billprater</t>
         </is>
       </c>
-      <c r="D33" s="36" t="inlineStr">
+      <c r="D33" s="38" t="inlineStr">
         <is>
           <t>Bill</t>
         </is>
       </c>
-      <c r="E33" s="36" t="inlineStr">
+      <c r="E33" s="38" t="inlineStr">
         <is>
           <t>Prater</t>
         </is>
       </c>
-      <c r="F33" s="36" t="inlineStr">
+      <c r="F33" s="38" t="inlineStr">
         <is>
           <t>Founder &amp; CEO | Mastermind Groups + Coaching + Team Building + Online Courses | Author – “How To Dominate Your Market”</t>
         </is>
       </c>
-      <c r="G33" s="36" t="inlineStr">
-        <is>
-          <t>Grande Seattle e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H33" s="36" t="inlineStr">
+      <c r="G33" s="38" t="inlineStr">
+        <is>
+          <t>Greater Seattle Area</t>
+        </is>
+      </c>
+      <c r="H33" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">WHAT I DO: Since 1999 I’ve helped Business Owners and Entrepreneurs in more than 50 different industries achieve real, measurable results using my unique approaches to grow revenue, increase cash flow and magnify business value.
 HOW I DO IT. I do this by incorporating several proprietary tools and techniques into the culture of the company and by empowering the team to manage the business. This consistently means the business owner’s personal efforts decline dramatically. 
@@ -1833,37 +1862,37 @@
       </c>
     </row>
     <row r="34" ht="409.5" customHeight="1">
-      <c r="B34" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C34" s="36" t="inlineStr">
+      <c r="B34" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C34" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/michaelarone</t>
         </is>
       </c>
-      <c r="D34" s="36" t="inlineStr">
+      <c r="D34" s="38" t="inlineStr">
         <is>
           <t>Michael</t>
         </is>
       </c>
-      <c r="E34" s="36" t="inlineStr">
+      <c r="E34" s="38" t="inlineStr">
         <is>
           <t>Arone</t>
         </is>
       </c>
-      <c r="F34" s="36" t="inlineStr">
+      <c r="F34" s="38" t="inlineStr">
         <is>
           <t>Chief Investment Strategist, Managing Director at State Street Global Advisors</t>
         </is>
       </c>
-      <c r="G34" s="36" t="inlineStr">
+      <c r="G34" s="38" t="inlineStr">
         <is>
           <t>Boston, Massachusetts</t>
         </is>
       </c>
-      <c r="H34" s="36" t="inlineStr">
+      <c r="H34" s="38" t="inlineStr">
         <is>
           <t>As a Managing Director of State Street Global Advisors and the Chief Investment Strategist for the US SPDR Business, I am responsible for expanding SSGA's footprint and thought leadership effort through frequent contributions to the financial news media, speaking engagements and client interactions. I am a frequent speaker at industry conferences and have authored several articles related to investment management practices. Here at SSGA I have previously served as the Global and EMEA Head of Portfolio Strategy as well as a senior portfolio manager in the Global Active Quantitative Equity Group.
 During my 20+-year career as a client-facing Investment Professional, I have served all major client segments, multiple asset classes and investment disciplines to help clients meet their long-term financial goals. I have substantial experience developing long-only and long-short quantitative strategies and managing investment portfolios using quantitative disciplines.
@@ -1872,38 +1901,38 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="204" customHeight="1">
-      <c r="B35" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C35" s="36" t="inlineStr">
+    <row r="35" ht="189" customHeight="1">
+      <c r="B35" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C35" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/srirampanyam</t>
         </is>
       </c>
-      <c r="D35" s="36" t="inlineStr">
+      <c r="D35" s="38" t="inlineStr">
         <is>
           <t>Sriram (Sri)</t>
         </is>
       </c>
-      <c r="E35" s="36" t="inlineStr">
+      <c r="E35" s="38" t="inlineStr">
         <is>
           <t>Panyam</t>
         </is>
       </c>
-      <c r="F35" s="36" t="inlineStr">
+      <c r="F35" s="38" t="inlineStr">
         <is>
           <t>Manager, Software Engineering at LinkedIn</t>
         </is>
       </c>
-      <c r="G35" s="36" t="inlineStr">
+      <c r="G35" s="38" t="inlineStr">
         <is>
           <t>Sunnyvale, California</t>
         </is>
       </c>
-      <c r="H35" s="36" t="inlineStr">
+      <c r="H35" s="38" t="inlineStr">
         <is>
           <t>I am passionate about building software and tools that power modern platforms and applications.  Over 15 years experience in wide ranging areas from embedded systems to gaming to mobile platforms to distributed systems and engineering leadership helps in understanding problems from various viewpoints and coming up with solutions (and sometimes problems) that are well thought out and impactful.
 Interests and Expertise: Scalable distributed systems, Service oriented architectures, Web services, API development and management, Language design.</t>
@@ -1911,37 +1940,37 @@
       </c>
     </row>
     <row r="36" ht="409.5" customHeight="1">
-      <c r="B36" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C36" s="36" t="inlineStr">
+      <c r="B36" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C36" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/dawsondavenport</t>
         </is>
       </c>
-      <c r="D36" s="36" t="inlineStr">
+      <c r="D36" s="38" t="inlineStr">
         <is>
           <t>Dawson</t>
         </is>
       </c>
-      <c r="E36" s="36" t="inlineStr">
+      <c r="E36" s="38" t="inlineStr">
         <is>
           <t>Davenport</t>
         </is>
       </c>
-      <c r="F36" s="36" t="inlineStr">
+      <c r="F36" s="38" t="inlineStr">
         <is>
           <t>President at TGG Realty</t>
         </is>
       </c>
-      <c r="G36" s="36" t="inlineStr">
+      <c r="G36" s="38" t="inlineStr">
         <is>
           <t>Costa Mesa, California</t>
         </is>
       </c>
-      <c r="H36" s="36" t="inlineStr">
+      <c r="H36" s="38" t="inlineStr">
         <is>
           <t>Dawson Davenport is an industry professional in business advisory and real estate services with over 35 years of experience encompassing REO/Receiver/Bankruptcy Assets, Real Estate Investments. Business Consulting, Business Operations,  Real Estate operations, Property Acquisition/Disposition, Property Renovation/Rehabilitation, and Asset Management.
 Mr. Davenport served as a key officer including President and Director of several real estate, real estate consulting and business consulting firms in Southern California.
@@ -1950,262 +1979,262 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="119.1" customHeight="1">
-      <c r="B37" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C37" s="36" t="inlineStr">
+    <row r="37" ht="110.25" customHeight="1">
+      <c r="B37" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C37" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/cameronpbean</t>
         </is>
       </c>
-      <c r="D37" s="36" t="inlineStr">
+      <c r="D37" s="38" t="inlineStr">
         <is>
           <t>Cameron</t>
         </is>
       </c>
-      <c r="E37" s="36" t="inlineStr">
+      <c r="E37" s="38" t="inlineStr">
         <is>
           <t>Bean</t>
         </is>
       </c>
-      <c r="F37" s="36" t="inlineStr">
+      <c r="F37" s="38" t="inlineStr">
         <is>
           <t>Assistant Vice President for Development &amp; Stewardship at Columbus State University</t>
         </is>
       </c>
-      <c r="G37" s="36" t="inlineStr">
-        <is>
-          <t>Columbus, Geórgia</t>
-        </is>
-      </c>
-      <c r="H37" s="36" t="inlineStr">
+      <c r="G37" s="38" t="inlineStr">
+        <is>
+          <t>Columbus, Georgia</t>
+        </is>
+      </c>
+      <c r="H37" s="38" t="inlineStr">
         <is>
           <t>Certified Fund Raising Executive with successful track record in lean, fast-paced non-profit and educational organizations. Expertise includes annual and capital fundraising campaigns, corporate and foundation relations, stewardship programs, public relations, creative solutions, board development and consensus building.</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="33.95" customHeight="1">
-      <c r="B38" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C38" s="36" t="inlineStr">
+    <row r="38" ht="31.5" customHeight="1">
+      <c r="B38" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C38" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/weiguo1</t>
         </is>
       </c>
-      <c r="D38" s="36" t="inlineStr">
+      <c r="D38" s="38" t="inlineStr">
         <is>
           <t>Wei</t>
         </is>
       </c>
-      <c r="E38" s="36" t="inlineStr">
+      <c r="E38" s="38" t="inlineStr">
         <is>
           <t>Guo</t>
         </is>
       </c>
-      <c r="F38" s="36" t="inlineStr">
+      <c r="F38" s="38" t="inlineStr">
         <is>
           <t>Analyst at Whale Rock Capital Management LLC</t>
         </is>
       </c>
-      <c r="G38" s="36" t="inlineStr">
+      <c r="G38" s="38" t="inlineStr">
         <is>
           <t>Boston, Massachusetts</t>
         </is>
       </c>
-      <c r="H38" s="36" t="inlineStr">
+      <c r="H38" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="153" customHeight="1">
-      <c r="B39" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C39" s="36" t="inlineStr">
+    <row r="39" ht="141.75" customHeight="1">
+      <c r="B39" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C39" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jameskenly</t>
         </is>
       </c>
-      <c r="D39" s="36" t="inlineStr">
+      <c r="D39" s="38" t="inlineStr">
         <is>
           <t>James</t>
         </is>
       </c>
-      <c r="E39" s="36" t="inlineStr">
+      <c r="E39" s="38" t="inlineStr">
         <is>
           <t>Kenly</t>
         </is>
       </c>
-      <c r="F39" s="36" t="inlineStr">
+      <c r="F39" s="38" t="inlineStr">
         <is>
           <t>Cultivating community at 8150'</t>
         </is>
       </c>
-      <c r="G39" s="36" t="inlineStr">
+      <c r="G39" s="38" t="inlineStr">
         <is>
           <t>Avon, Colorado</t>
         </is>
       </c>
-      <c r="H39" s="36" t="inlineStr">
+      <c r="H39" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Self-actualizing business leader with a passion for the mountains, business administration and community development. A Lean and creative systems thinker thriving at the intersection of what is and what is possible. Dedicated to facilitating the connection between people and purpose through integrated business systems that reinforce a compelling brand promise.
 </t>
         </is>
       </c>
     </row>
-    <row r="40" ht="186.95" customHeight="1">
-      <c r="B40" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C40" s="36" t="inlineStr">
+    <row r="40" ht="157.5" customHeight="1">
+      <c r="B40" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C40" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/joshrubinca</t>
         </is>
       </c>
-      <c r="D40" s="36" t="inlineStr">
+      <c r="D40" s="38" t="inlineStr">
         <is>
           <t>Josh</t>
         </is>
       </c>
-      <c r="E40" s="36" t="inlineStr">
+      <c r="E40" s="38" t="inlineStr">
         <is>
           <t>Rubin</t>
         </is>
       </c>
-      <c r="F40" s="36" t="inlineStr">
+      <c r="F40" s="38" t="inlineStr">
         <is>
           <t>Ask me how you can meet your 2020 business goals through strategic marketing!</t>
         </is>
       </c>
-      <c r="G40" s="36" t="inlineStr">
+      <c r="G40" s="38" t="inlineStr">
         <is>
           <t>Sacramento, California</t>
         </is>
       </c>
-      <c r="H40" s="36" t="inlineStr">
+      <c r="H40" s="38" t="inlineStr">
         <is>
           <t>I own Post Modern Marketing - a top digital marketing firm with locations in Sacramento, San Diego, Reno and Lexington. We were the region's 4th fastest growing company in 2018, 6th in 2019, and have been awarded as a top firm by several agencies.
 Specialties: Web development, SEO, web marketing, identity/brand development, process architect.  Using modern technology without losing focus on customer service and basic marketing principals.</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="153" customHeight="1">
-      <c r="B41" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C41" s="36" t="inlineStr">
+    <row r="41" ht="141.75" customHeight="1">
+      <c r="B41" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C41" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/brianbehlendorf</t>
         </is>
       </c>
-      <c r="D41" s="36" t="inlineStr">
+      <c r="D41" s="38" t="inlineStr">
         <is>
           <t>Brian</t>
         </is>
       </c>
-      <c r="E41" s="36" t="inlineStr">
+      <c r="E41" s="38" t="inlineStr">
         <is>
           <t>Behlendorf</t>
         </is>
       </c>
-      <c r="F41" s="36" t="inlineStr">
+      <c r="F41" s="38" t="inlineStr">
         <is>
           <t>Executive Director of the Hyperledger Project</t>
         </is>
       </c>
-      <c r="G41" s="36" t="inlineStr">
-        <is>
-          <t>Baía de São Francisco e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H41" s="36" t="inlineStr">
+      <c r="G41" s="38" t="inlineStr">
+        <is>
+          <t>San Francisco Bay Area</t>
+        </is>
+      </c>
+      <c r="H41" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">I've dedicated my career to connecting and empowering the Free Software and Open Source community to solve hard technology problems and have a positive societal impact.  I've done this wearing many different hats - as a startup company founder, as an advisor to the U.S. government, as a board member at various non-profits and consortia, as a YGL and employee of the World Economic Forum, and as an investor.  </t>
         </is>
       </c>
     </row>
-    <row r="42" ht="51" customHeight="1">
-      <c r="B42" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C42" s="36" t="inlineStr">
+    <row r="42" ht="47.25" customHeight="1">
+      <c r="B42" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C42" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/willjohnson</t>
         </is>
       </c>
-      <c r="D42" s="36" t="inlineStr">
+      <c r="D42" s="38" t="inlineStr">
         <is>
           <t>Will</t>
         </is>
       </c>
-      <c r="E42" s="36" t="inlineStr">
+      <c r="E42" s="38" t="inlineStr">
         <is>
           <t>Johnson</t>
         </is>
       </c>
-      <c r="F42" s="36" t="inlineStr">
+      <c r="F42" s="38" t="inlineStr">
         <is>
           <t>Director Of Software Engineering, Search at ServiceNow</t>
         </is>
       </c>
-      <c r="G42" s="36" t="inlineStr">
-        <is>
-          <t>Grande Boston e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H42" s="36" t="inlineStr">
+      <c r="G42" s="38" t="inlineStr">
+        <is>
+          <t>Greater Boston Area</t>
+        </is>
+      </c>
+      <c r="H42" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="43" ht="204" customHeight="1">
-      <c r="B43" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C43" s="36" t="inlineStr">
+    <row r="43" ht="173.25" customHeight="1">
+      <c r="B43" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C43" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/petejadavies</t>
         </is>
       </c>
-      <c r="D43" s="36" t="inlineStr">
+      <c r="D43" s="38" t="inlineStr">
         <is>
           <t>Pete</t>
         </is>
       </c>
-      <c r="E43" s="36" t="inlineStr">
+      <c r="E43" s="38" t="inlineStr">
         <is>
           <t>Davies</t>
         </is>
       </c>
-      <c r="F43" s="36" t="inlineStr">
+      <c r="F43" s="38" t="inlineStr">
         <is>
           <t>Recovering journalist.</t>
         </is>
       </c>
-      <c r="G43" s="36" t="inlineStr">
-        <is>
-          <t>Baía de São Francisco e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H43" s="36" t="inlineStr">
+      <c r="G43" s="38" t="inlineStr">
+        <is>
+          <t>San Francisco Bay Area</t>
+        </is>
+      </c>
+      <c r="H43" s="38" t="inlineStr">
         <is>
           <t>I lead the Identity, Search, and Content teams at LinkedIn, where we are enabling our members to build and engage with communities that help them to become more productive and successful.
 Formerly... Product Lead and Product Scientist (Medium); Growth &amp; Analytics Lead and Product Lead (Automattic/WordPress.com); General Manager (TerraPass); Journalist &amp; Senior Producer (BBC Radio).
@@ -2213,76 +2242,76 @@
         </is>
       </c>
     </row>
-    <row r="44" ht="50.1" customHeight="1">
-      <c r="B44" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C44" s="36" t="inlineStr">
+    <row r="44" ht="173.25" customHeight="1">
+      <c r="B44" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C44" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/shyamnagarajan</t>
         </is>
       </c>
-      <c r="D44" s="36" t="inlineStr">
+      <c r="D44" s="38" t="inlineStr">
         <is>
           <t>Shyam</t>
         </is>
       </c>
-      <c r="E44" s="36" t="inlineStr">
+      <c r="E44" s="38" t="inlineStr">
         <is>
           <t>Nagarajan</t>
         </is>
       </c>
-      <c r="F44" s="36" t="inlineStr">
+      <c r="F44" s="38" t="inlineStr">
         <is>
           <t>Director, Go To Market Blockchain Networks at IBM Services</t>
         </is>
       </c>
-      <c r="G44" s="36" t="inlineStr">
-        <is>
-          <t>Cidade de Nova Iorque e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H44" s="36" t="inlineStr">
+      <c r="G44" s="38" t="inlineStr">
+        <is>
+          <t>Greater New York City Area</t>
+        </is>
+      </c>
+      <c r="H44" s="38" t="inlineStr">
         <is>
           <t>Experienced business growth (sales and technology) executive with sharp acumen for achieving business results.  Creative, resourceful and strategic in pursuing new initiatives from concept to completion.  High performance team leader with proven track record in driving change and managing growth.
 software portfolio, software revenue, sales leader, sales professionals, process management, overachieved, application server, growth markets, high performance, sales management and execution</t>
         </is>
       </c>
     </row>
-    <row r="45" ht="255" customHeight="1">
-      <c r="B45" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C45" s="36" t="inlineStr">
+    <row r="45" ht="236.25" customHeight="1">
+      <c r="B45" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C45" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/leopmcguire</t>
         </is>
       </c>
-      <c r="D45" s="36" t="inlineStr">
+      <c r="D45" s="38" t="inlineStr">
         <is>
           <t>Leo P.</t>
         </is>
       </c>
-      <c r="E45" s="36" t="inlineStr">
+      <c r="E45" s="38" t="inlineStr">
         <is>
           <t>McGuire, MBA</t>
         </is>
       </c>
-      <c r="F45" s="36" t="inlineStr">
+      <c r="F45" s="38" t="inlineStr">
         <is>
           <t>Head of Security/Dir. of Risk Management</t>
         </is>
       </c>
-      <c r="G45" s="36" t="inlineStr">
-        <is>
-          <t>Paramus, Nova Jersey</t>
-        </is>
-      </c>
-      <c r="H45" s="36" t="inlineStr">
+      <c r="G45" s="38" t="inlineStr">
+        <is>
+          <t>Paramus, New Jersey</t>
+        </is>
+      </c>
+      <c r="H45" s="38" t="inlineStr">
         <is>
           <t>An experienced chief executive who successfully led a large governmental organization ($58M/550 employees), that enhanced revenues and contained costs while developing innovative solutions to complex issues. 
 Solution-oriented leadership understanding the value of team building towards achieving strategic goals on behalf of the organization.
@@ -2290,75 +2319,75 @@
         </is>
       </c>
     </row>
-    <row r="46" ht="51" customHeight="1">
-      <c r="B46" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C46" s="34" t="inlineStr">
+    <row r="46" ht="47.25" customHeight="1">
+      <c r="B46" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C46" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/kristalane</t>
         </is>
       </c>
-      <c r="D46" s="36" t="inlineStr">
+      <c r="D46" s="38" t="inlineStr">
         <is>
           <t>Krista</t>
         </is>
       </c>
-      <c r="E46" s="36" t="inlineStr">
+      <c r="E46" s="38" t="inlineStr">
         <is>
           <t>Lane</t>
         </is>
       </c>
-      <c r="F46" s="36" t="inlineStr">
+      <c r="F46" s="38" t="inlineStr">
         <is>
           <t>Executive Producer of Special Projects at CBS4/FOX59</t>
         </is>
       </c>
-      <c r="G46" s="36" t="inlineStr">
+      <c r="G46" s="38" t="inlineStr">
         <is>
           <t>Indianapolis, Indiana</t>
         </is>
       </c>
-      <c r="H46" s="36" t="inlineStr">
+      <c r="H46" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
     <row r="47" ht="409.5" customHeight="1">
-      <c r="B47" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C47" s="34" t="inlineStr">
+      <c r="B47" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C47" s="36" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/schmidtmaxr</t>
         </is>
       </c>
-      <c r="D47" s="36" t="inlineStr">
+      <c r="D47" s="38" t="inlineStr">
         <is>
           <t>Max</t>
         </is>
       </c>
-      <c r="E47" s="36" t="inlineStr">
+      <c r="E47" s="38" t="inlineStr">
         <is>
           <t>Schmidt</t>
         </is>
       </c>
-      <c r="F47" s="36" t="inlineStr">
+      <c r="F47" s="38" t="inlineStr">
         <is>
           <t>Chief Information Officer at The World</t>
         </is>
       </c>
-      <c r="G47" s="36" t="inlineStr">
-        <is>
-          <t>Miami/Fort Lauderdale e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H47" s="36" t="inlineStr">
+      <c r="G47" s="38" t="inlineStr">
+        <is>
+          <t>Miami/Fort Lauderdale Area</t>
+        </is>
+      </c>
+      <c r="H47" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Information technology and business leader with extensive travel and hospitality experience.  Adept at implementing innovative technology that breaks legacy barriers to enhance customer experience, reduce cost and improve operational efficiencies. Implements an engaging and culture-based leadership style with the proven ability to motivate and perform at high levels of productivity.  Proven track record with managing multi-million dollar budgets and driving millions of incremental revenue through the deployment of technology.  Experience in managing global IT operations consisting of over 26 shoreside corporate offices and 42 ships located in the USA, Latin America, Asia and Europe. 
@@ -2378,38 +2407,38 @@
         </is>
       </c>
     </row>
-    <row r="48" ht="237.95" customHeight="1">
-      <c r="B48" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C48" s="36" t="inlineStr">
+    <row r="48" ht="220.5" customHeight="1">
+      <c r="B48" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C48" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/nedstaebler</t>
         </is>
       </c>
-      <c r="D48" s="36" t="inlineStr">
+      <c r="D48" s="38" t="inlineStr">
         <is>
           <t>Ned</t>
         </is>
       </c>
-      <c r="E48" s="36" t="inlineStr">
+      <c r="E48" s="38" t="inlineStr">
         <is>
           <t>Staebler</t>
         </is>
       </c>
-      <c r="F48" s="36" t="inlineStr">
+      <c r="F48" s="38" t="inlineStr">
         <is>
           <t>Vice President for Economic Development at Wayne State University and President and CEO of TechTown</t>
         </is>
       </c>
-      <c r="G48" s="36" t="inlineStr">
+      <c r="G48" s="38" t="inlineStr">
         <is>
           <t>Ann Arbor, Michigan</t>
         </is>
       </c>
-      <c r="H48" s="36" t="inlineStr">
+      <c r="H48" s="38" t="inlineStr">
         <is>
           <t>Entrepreneurial leader experienced in crafting and implementing statewide innovation-based economic development policy and internationally recognized best practices in community-based inclusive economic development.
 Extensive experience building and leading successful teams of talented vice president and director level managers in both startup and Fortune 150 business settings. Far-reaching connections in the business community in Southeast Michigan and across the state. Proven track record of building consensus and strategic coalitions with local, statewide and regional economic development and industry groups.</t>
@@ -2417,37 +2446,37 @@
       </c>
     </row>
     <row r="49" ht="409.5" customHeight="1">
-      <c r="B49" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C49" s="36" t="inlineStr">
+      <c r="B49" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C49" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/donbora</t>
         </is>
       </c>
-      <c r="D49" s="36" t="inlineStr">
+      <c r="D49" s="38" t="inlineStr">
         <is>
           <t>Don</t>
         </is>
       </c>
-      <c r="E49" s="36" t="inlineStr">
+      <c r="E49" s="38" t="inlineStr">
         <is>
           <t>Bora</t>
         </is>
       </c>
-      <c r="F49" s="36" t="inlineStr">
+      <c r="F49" s="38" t="inlineStr">
         <is>
           <t>Co-Founder and Principal of Technology Eight Bit Studios. Public Speaker</t>
         </is>
       </c>
-      <c r="G49" s="36" t="inlineStr">
+      <c r="G49" s="38" t="inlineStr">
         <is>
           <t>Chicago, Illinois</t>
         </is>
       </c>
-      <c r="H49" s="36" t="inlineStr">
+      <c r="H49" s="38" t="inlineStr">
         <is>
           <t>**Recruiters**
 And I say this with all of the love in my heart: I am currently partner/principal in technology and co-founder of Eight Bit Studios where I help run the company and oversee all things tech. I am not leaving my current positions. Thank you for your interest insofar as reading this and good luck in your search. 
@@ -2474,37 +2503,37 @@
       </c>
     </row>
     <row r="50" ht="409.5" customHeight="1">
-      <c r="B50" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C50" s="36" t="inlineStr">
+      <c r="B50" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C50" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/lynndessert</t>
         </is>
       </c>
-      <c r="D50" s="36" t="inlineStr">
+      <c r="D50" s="38" t="inlineStr">
         <is>
           <t>Lynn</t>
         </is>
       </c>
-      <c r="E50" s="36" t="inlineStr">
+      <c r="E50" s="38" t="inlineStr">
         <is>
           <t>Dessert MBA, MCC</t>
         </is>
       </c>
-      <c r="F50" s="36" t="inlineStr">
+      <c r="F50" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">Master Certified Coach | Executive Leadership Coach | Mentor Coach | Past President ICF CAC | Speaker | 704-412-2852 </t>
         </is>
       </c>
-      <c r="G50" s="36" t="inlineStr">
-        <is>
-          <t>Charlotte, Carolina do Norte e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H50" s="36" t="inlineStr">
+      <c r="G50" s="38" t="inlineStr">
+        <is>
+          <t>Charlotte, North Carolina Area</t>
+        </is>
+      </c>
+      <c r="H50" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">If I can be of service to your professional or personal development, contact me at 704-412-2852 or https://live.vcita.com/site/lynndessert.
 Executive Coaching
@@ -2531,75 +2560,75 @@
         </is>
       </c>
     </row>
-    <row r="51" ht="84.95" customHeight="1">
-      <c r="B51" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C51" s="36" t="inlineStr">
+    <row r="51" ht="78.75" customHeight="1">
+      <c r="B51" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C51" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/haileyhu</t>
         </is>
       </c>
-      <c r="D51" s="36" t="inlineStr">
+      <c r="D51" s="38" t="inlineStr">
         <is>
           <t>Hailey</t>
         </is>
       </c>
-      <c r="E51" s="36" t="inlineStr">
+      <c r="E51" s="38" t="inlineStr">
         <is>
           <t>Hu</t>
         </is>
       </c>
-      <c r="F51" s="36" t="inlineStr">
+      <c r="F51" s="38" t="inlineStr">
         <is>
           <t>Investment Director at AiiM Partners</t>
         </is>
       </c>
-      <c r="G51" s="36" t="inlineStr">
-        <is>
-          <t>Baía de São Francisco e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H51" s="36" t="inlineStr">
+      <c r="G51" s="38" t="inlineStr">
+        <is>
+          <t>San Francisco Bay Area</t>
+        </is>
+      </c>
+      <c r="H51" s="38" t="inlineStr">
         <is>
           <t>Investing in early-stage startups addressing climate change, sustainability, and access.  Experience in investing, strategy, operations, and business development globally. INSEAD MBA, Wharton undergrad, San Diego native.</t>
         </is>
       </c>
     </row>
-    <row r="52" ht="33.95" customHeight="1">
-      <c r="B52" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C52" s="36" t="inlineStr">
+    <row r="52" ht="31.5" customHeight="1">
+      <c r="B52" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C52" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/warald</t>
         </is>
       </c>
-      <c r="D52" s="36" t="inlineStr">
+      <c r="D52" s="38" t="inlineStr">
         <is>
           <t>Warald</t>
         </is>
       </c>
-      <c r="E52" s="36" t="inlineStr">
+      <c r="E52" s="38" t="inlineStr">
         <is>
           <t>一亩三分地</t>
         </is>
       </c>
-      <c r="F52" s="36" t="inlineStr">
+      <c r="F52" s="38" t="inlineStr">
         <is>
           <t>CEO at 1Point3Acres, LLC</t>
         </is>
       </c>
-      <c r="G52" s="36" t="inlineStr">
+      <c r="G52" s="38" t="inlineStr">
         <is>
           <t>Las Vegas, Nevada</t>
         </is>
       </c>
-      <c r="H52" s="36" t="inlineStr">
+      <c r="H52" s="38" t="inlineStr">
         <is>
           <t xml:space="preserve">一亩三分地伴你一起成长
 Together. Aim higher. Achieve more. </t>
@@ -2607,37 +2636,37 @@
       </c>
     </row>
     <row r="53" ht="409.5" customHeight="1">
-      <c r="B53" s="35" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C53" s="36" t="inlineStr">
+      <c r="B53" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C53" s="38" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/katiesowieja</t>
         </is>
       </c>
-      <c r="D53" s="36" t="inlineStr">
+      <c r="D53" s="38" t="inlineStr">
         <is>
           <t>Katie</t>
         </is>
       </c>
-      <c r="E53" s="36" t="inlineStr">
+      <c r="E53" s="38" t="inlineStr">
         <is>
           <t>Sowieja</t>
         </is>
       </c>
-      <c r="F53" s="36" t="inlineStr">
+      <c r="F53" s="38" t="inlineStr">
         <is>
           <t>Director of Brand Marketing</t>
         </is>
       </c>
-      <c r="G53" s="36" t="inlineStr">
-        <is>
-          <t>Grande Minneapolis-St. Paul e Região, Estados Unidos</t>
-        </is>
-      </c>
-      <c r="H53" s="36" t="inlineStr">
+      <c r="G53" s="38" t="inlineStr">
+        <is>
+          <t>Greater Minneapolis-St. Paul Area</t>
+        </is>
+      </c>
+      <c r="H53" s="38" t="inlineStr">
         <is>
           <t>Delivering Growth Through Insight-Driven Strategy
 Accomplished marketing leader with both corporate and agency experience. Proven ability to develop insight-driven, innovative strategic marketing plans that facilitate business growth.
@@ -2648,7 +2677,101 @@
         </is>
       </c>
     </row>
-    <row r="54"/>
+    <row r="54" ht="63" customHeight="1">
+      <c r="B54" s="37" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C54" s="36" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/rodrigo-miksian-magaldi</t>
+        </is>
+      </c>
+      <c r="D54" s="38" t="inlineStr">
+        <is>
+          <t>Rodrigo</t>
+        </is>
+      </c>
+      <c r="E54" s="38" t="inlineStr">
+        <is>
+          <t>Miksian Magaldi</t>
+        </is>
+      </c>
+      <c r="F54" s="38" t="inlineStr">
+        <is>
+          <t>Gerente de tecnologia na Poli Júnior</t>
+        </is>
+      </c>
+      <c r="G54" s="38" t="inlineStr">
+        <is>
+          <t>São Paulo, São Paulo, Brazil</t>
+        </is>
+      </c>
+      <c r="H54" s="38" t="inlineStr">
+        <is>
+          <t>Estudante do 7º semestre de Engenharia Elétrica (ênfase em computação) na Escola Politécnica da USP, e Gerente de Tecnologia da Poli Júnior. Desenvolvedor aficionado e apaixonado por dados.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" ht="63" customHeight="1">
+      <c r="B55" s="37" t="inlineStr">
+        <is>
+          <t>Sim (Cópia)</t>
+        </is>
+      </c>
+      <c r="C55" s="36" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/rodrigo-miksian-magaldi</t>
+        </is>
+      </c>
+      <c r="D55" s="38" t="inlineStr">
+        <is>
+          <t>Rodrigo</t>
+        </is>
+      </c>
+      <c r="E55" s="38" t="inlineStr">
+        <is>
+          <t>Miksian Magaldi</t>
+        </is>
+      </c>
+      <c r="F55" s="38" t="inlineStr">
+        <is>
+          <t>Gerente de tecnologia na Poli Júnior</t>
+        </is>
+      </c>
+      <c r="G55" s="38" t="inlineStr">
+        <is>
+          <t>São Paulo, São Paulo, Brazil</t>
+        </is>
+      </c>
+      <c r="H55" s="38" t="inlineStr">
+        <is>
+          <t>Estudante do 7º semestre de Engenharia Elétrica (ênfase em computação) na Escola Politécnica da USP, e Gerente de Tecnologia da Poli Júnior. Desenvolvedor aficionado e apaixonado por dados.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" s="37" t="inlineStr">
+        <is>
+          <t>Não é uma pessoa</t>
+        </is>
+      </c>
+      <c r="C56" s="36" t="inlineStr">
+        <is>
+          <t>https://stackoverflow.com/questions/48030717/scrapy-404-error-http-status-code-is-not-handled-or-not-allowed</t>
+        </is>
+      </c>
+      <c r="D56" s="38" t="n"/>
+      <c r="E56" s="38" t="n"/>
+      <c r="F56" s="38" t="n"/>
+      <c r="G56" s="38" t="n"/>
+      <c r="H56" s="38" t="n"/>
+    </row>
+    <row r="57"/>
+    <row r="60">
+      <c r="H60" s="11" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="F5:H7"/>
@@ -2659,627 +2782,175 @@
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D6">
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="0">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="1">
       <formula>"Sim"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
-      <formula>"Não é uma pessoa"</formula>
+  <conditionalFormatting sqref="B4 B9:B1048576">
+    <cfRule type="containsText" priority="2" operator="containsText" dxfId="10" text="Não">
+      <formula>NOT(ISERROR(SEARCH("Não",B4)))</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1">
-      <formula>"Sim"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" dxfId="0">
-      <formula>"Não"</formula>
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="9" text="Sim">
+      <formula>NOT(ISERROR(SEARCH("Sim",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId589"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId590"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId591"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId592"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId593"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId594"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId595"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId596"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId597"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId598"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId599"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId600"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -3289,10 +2960,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:G17"/>
+  <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.875" defaultRowHeight="15.75" outlineLevelCol="0"/>
@@ -3304,8 +2975,8 @@
     <col width="10.875" customWidth="1" style="3" min="5" max="5"/>
     <col width="13" customWidth="1" style="3" min="6" max="6"/>
     <col width="64.875" customWidth="1" style="1" min="7" max="7"/>
-    <col width="10.875" customWidth="1" style="1" min="8" max="65"/>
-    <col width="10.875" customWidth="1" style="1" min="66" max="16384"/>
+    <col width="10.875" customWidth="1" style="1" min="8" max="71"/>
+    <col width="10.875" customWidth="1" style="1" min="72" max="16384"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -3341,426 +3012,366 @@
       </c>
     </row>
     <row r="3" ht="31.5" customHeight="1">
-      <c r="B3" s="36" t="inlineStr">
+      <c r="B3" s="38" t="inlineStr">
         <is>
           <t>leslie.brown.comm@gmail.com</t>
         </is>
       </c>
-      <c r="C3" s="36" t="inlineStr">
+      <c r="C3" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D3" s="36" t="n">
-        <v>29</v>
-      </c>
-      <c r="E3" s="36" t="inlineStr">
+      <c r="D3" s="38" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F3" s="36" t="inlineStr">
+      <c r="F3" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G3" s="37" t="inlineStr">
+      <c r="G3" s="39" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="4" ht="31.5" customHeight="1">
-      <c r="B4" s="36" t="inlineStr">
+      <c r="B4" s="38" t="inlineStr">
         <is>
           <t>asdrubal_dos_santos@gmail.com</t>
         </is>
       </c>
-      <c r="C4" s="36" t="inlineStr">
+      <c r="C4" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D4" s="36" t="n">
-        <v>49</v>
-      </c>
-      <c r="E4" s="36" t="inlineStr">
+      <c r="D4" s="38" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F4" s="36" t="inlineStr">
+      <c r="F4" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G4" s="37" t="inlineStr">
+      <c r="G4" s="39" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="5" ht="31.5" customHeight="1">
-      <c r="B5" s="34" t="inlineStr">
+      <c r="B5" s="36" t="inlineStr">
         <is>
           <t>pedro_alcantara_siveira@gmail.com</t>
         </is>
       </c>
-      <c r="C5" s="36" t="inlineStr">
+      <c r="C5" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D5" s="36" t="n">
-        <v>59</v>
-      </c>
-      <c r="E5" s="36" t="inlineStr">
+      <c r="D5" s="38" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F5" s="36" t="inlineStr">
+      <c r="F5" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G5" s="37" t="inlineStr">
+      <c r="G5" s="39" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="6" ht="31.5" customHeight="1">
-      <c r="B6" s="36" t="inlineStr">
+      <c r="B6" s="38" t="inlineStr">
         <is>
           <t>cleber_cunha_dasilva@gmail.com</t>
         </is>
       </c>
-      <c r="C6" s="36" t="inlineStr">
+      <c r="C6" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D6" s="36" t="n">
-        <v>54</v>
-      </c>
-      <c r="E6" s="36" t="inlineStr">
+      <c r="D6" s="38" t="n">
+        <v>14</v>
+      </c>
+      <c r="E6" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F6" s="36" t="inlineStr">
+      <c r="F6" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G6" s="37" t="inlineStr">
+      <c r="G6" s="39" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="7" ht="31.5" customHeight="1">
-      <c r="B7" s="36" t="inlineStr">
+      <c r="B7" s="38" t="inlineStr">
         <is>
           <t>emerencia_silveira@gmail.com</t>
         </is>
       </c>
-      <c r="C7" s="36" t="inlineStr">
+      <c r="C7" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D7" s="36" t="n">
-        <v>45</v>
-      </c>
-      <c r="E7" s="36" t="inlineStr">
+      <c r="D7" s="38" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F7" s="36" t="inlineStr">
+      <c r="F7" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G7" s="37" t="inlineStr">
+      <c r="G7" s="39" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="8" ht="31.5" customHeight="1">
-      <c r="B8" s="36" t="inlineStr">
+      <c r="B8" s="38" t="inlineStr">
         <is>
           <t>ezequiel_valentim@gmail.com</t>
         </is>
       </c>
-      <c r="C8" s="36" t="inlineStr">
+      <c r="C8" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D8" s="36" t="n">
-        <v>33</v>
-      </c>
-      <c r="E8" s="36" t="inlineStr">
+      <c r="D8" s="38" t="n">
+        <v>13</v>
+      </c>
+      <c r="E8" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F8" s="36" t="inlineStr">
+      <c r="F8" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G8" s="37" t="inlineStr">
+      <c r="G8" s="39" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="9" ht="31.5" customHeight="1">
-      <c r="B9" s="36" t="inlineStr">
+      <c r="B9" s="38" t="inlineStr">
         <is>
           <t>ermedovaldo_clemente@gmail.com</t>
         </is>
       </c>
-      <c r="C9" s="36" t="inlineStr">
+      <c r="C9" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D9" s="36" t="n">
-        <v>44</v>
-      </c>
-      <c r="E9" s="36" t="inlineStr">
+      <c r="D9" s="38" t="n">
+        <v>14</v>
+      </c>
+      <c r="E9" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F9" s="36" t="inlineStr">
+      <c r="F9" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G9" s="37" t="inlineStr">
+      <c r="G9" s="39" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="10" ht="31.5" customHeight="1">
-      <c r="B10" s="36" t="inlineStr">
+      <c r="B10" s="38" t="inlineStr">
         <is>
           <t>jonas_pedroso@gmail.com</t>
         </is>
       </c>
-      <c r="C10" s="36" t="inlineStr">
+      <c r="C10" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D10" s="36" t="n">
-        <v>73</v>
-      </c>
-      <c r="E10" s="36" t="inlineStr">
+      <c r="D10" s="38" t="n">
+        <v>13</v>
+      </c>
+      <c r="E10" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F10" s="36" t="inlineStr">
+      <c r="F10" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G10" s="36" t="inlineStr">
+      <c r="G10" s="38" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="11" ht="31.5" customHeight="1">
-      <c r="B11" s="36" t="inlineStr">
+      <c r="B11" s="38" t="inlineStr">
         <is>
           <t>nivaldo_osvaldi@gmail.com</t>
         </is>
       </c>
-      <c r="C11" s="36" t="inlineStr">
+      <c r="C11" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D11" s="36" t="n">
-        <v>32</v>
-      </c>
-      <c r="E11" s="36" t="inlineStr">
+      <c r="D11" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F11" s="36" t="inlineStr">
+      <c r="F11" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G11" s="36" t="inlineStr">
+      <c r="G11" s="38" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="12" ht="31.5" customHeight="1">
-      <c r="B12" s="34" t="inlineStr">
+      <c r="B12" s="36" t="inlineStr">
         <is>
           <t>pedro_pedroso@gmail.com</t>
         </is>
       </c>
-      <c r="C12" s="36" t="inlineStr">
+      <c r="C12" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D12" s="36" t="n">
-        <v>55</v>
-      </c>
-      <c r="E12" s="36" t="inlineStr">
+      <c r="D12" s="38" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F12" s="36" t="inlineStr">
+      <c r="F12" s="38" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G12" s="36" t="inlineStr">
+      <c r="G12" s="38" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
     <row r="13" ht="31.5" customHeight="1">
-      <c r="B13" s="36" t="inlineStr">
+      <c r="B13" s="38" t="inlineStr">
         <is>
           <t>deodoro_fonseca@gmail.com</t>
         </is>
       </c>
-      <c r="C13" s="36" t="inlineStr">
+      <c r="C13" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D13" s="36" t="n">
-        <v>6</v>
-      </c>
-      <c r="E13" s="36" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F13" s="36" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="G13" s="36" t="inlineStr">
+      <c r="D13" s="38" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" s="38" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F13" s="38" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="G13" s="38" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
     <row r="14" ht="31.5" customHeight="1">
-      <c r="B14" s="36" t="inlineStr">
+      <c r="B14" s="38" t="inlineStr">
         <is>
           <t>pedro_alvarez@gmail.com</t>
         </is>
       </c>
-      <c r="C14" s="36" t="inlineStr">
+      <c r="C14" s="38" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D14" s="36" t="n">
-        <v>5</v>
-      </c>
-      <c r="E14" s="36" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F14" s="36" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="G14" s="36" t="inlineStr">
-        <is>
-          <t>---</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="31.5" customHeight="1">
-      <c r="B15" s="36" t="inlineStr">
-        <is>
-          <t>pedro_pires_pinheiro@gmail.com</t>
-        </is>
-      </c>
-      <c r="C15" s="36" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D15" s="36" t="n">
-        <v>4</v>
-      </c>
-      <c r="E15" s="36" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F15" s="36" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="G15" s="36" t="inlineStr">
-        <is>
-          <t>---</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="31.5" customHeight="1">
-      <c r="B16" s="36" t="inlineStr">
-        <is>
-          <t>hermedovaldo_da_silva@gmail.com</t>
-        </is>
-      </c>
-      <c r="C16" s="36" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D16" s="36" t="n">
-        <v>4</v>
-      </c>
-      <c r="E16" s="36" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F16" s="36" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="G16" s="36" t="inlineStr">
-        <is>
-          <t>---</t>
-        </is>
-      </c>
-    </row>
-    <row r="17"/>
+      <c r="D14" s="38" t="n">
+        <v>11</v>
+      </c>
+      <c r="E14" s="38" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F14" s="38" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="G14" s="38" t="inlineStr">
+        <is>
+          <t>Conta pede uma verificação se é um robô. Acesse o linkedin com essa conta e resolva o captcha.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15"/>
   </sheetData>
   <conditionalFormatting sqref="G2 F1:F3 F13:F1048576">
     <cfRule type="cellIs" priority="8" operator="equal" dxfId="1">
@@ -3798,106 +3409,26 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId99"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId100"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
add mac os executable
</commit_message>
<xml_diff>
--- a/windows_executable/Links.xlsx
+++ b/windows_executable/Links.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="20940" yWindow="2295" windowWidth="15645" windowHeight="12735" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1520" yWindow="1520" windowWidth="23180" windowHeight="13700" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Links" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="14">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -77,29 +77,10 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="18"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <scheme val="minor"/>
-    </font>
-    <font/>
-    <font>
       <sz val="18"/>
     </font>
   </fonts>
@@ -111,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -255,27 +236,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="00000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
@@ -304,14 +270,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -319,16 +282,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -358,28 +321,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -472,11 +419,20 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
+        <patternFill>
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
@@ -486,7 +442,7 @@
         <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -817,40 +773,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H60"/>
+  <dimension ref="B2:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" zoomScale="35" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.875" defaultRowHeight="15.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col width="10.875" customWidth="1" style="23" min="1" max="1"/>
-    <col width="17" customWidth="1" style="23" min="2" max="2"/>
-    <col width="62.875" customWidth="1" style="23" min="3" max="3"/>
-    <col width="16" customWidth="1" style="23" min="4" max="4"/>
-    <col width="18.375" customWidth="1" style="23" min="5" max="5"/>
-    <col width="23.125" customWidth="1" style="23" min="6" max="6"/>
-    <col width="32.125" customWidth="1" style="23" min="7" max="7"/>
-    <col width="46.625" customWidth="1" style="23" min="8" max="8"/>
-    <col width="10.875" customWidth="1" style="23" min="9" max="76"/>
-    <col width="10.875" customWidth="1" style="23" min="77" max="16384"/>
+    <col width="10.83203125" customWidth="1" style="22" min="1" max="1"/>
+    <col width="15" customWidth="1" style="22" min="2" max="2"/>
+    <col width="62.83203125" customWidth="1" style="22" min="3" max="3"/>
+    <col width="16" customWidth="1" style="22" min="4" max="4"/>
+    <col width="18.33203125" customWidth="1" style="22" min="5" max="5"/>
+    <col width="23.1640625" customWidth="1" style="22" min="6" max="6"/>
+    <col width="32.1640625" customWidth="1" style="22" min="7" max="7"/>
+    <col width="46.6640625" customWidth="1" style="22" min="8" max="8"/>
+    <col width="10.83203125" customWidth="1" style="22" min="9" max="72"/>
+    <col width="10.83203125" customWidth="1" style="22" min="73" max="16384"/>
   </cols>
   <sheetData>
     <row r="2" ht="45" customHeight="1">
-      <c r="B2" s="32" t="inlineStr">
+      <c r="B2" s="31" t="inlineStr">
         <is>
           <t>TABELA DE OBTENÇÃO DE DADOS</t>
         </is>
       </c>
-      <c r="C2" s="29" t="n"/>
-      <c r="D2" s="29" t="n"/>
-      <c r="E2" s="29" t="n"/>
-      <c r="F2" s="29" t="n"/>
-      <c r="G2" s="29" t="n"/>
-      <c r="H2" s="30" t="n"/>
-    </row>
-    <row r="3" ht="26.1" customHeight="1">
+      <c r="C2" s="28" t="n"/>
+      <c r="D2" s="28" t="n"/>
+      <c r="E2" s="28" t="n"/>
+      <c r="F2" s="28" t="n"/>
+      <c r="G2" s="28" t="n"/>
+      <c r="H2" s="29" t="n"/>
+    </row>
+    <row r="3" ht="26" customHeight="1">
       <c r="B3" s="6" t="n"/>
       <c r="C3" s="7" t="n"/>
       <c r="D3" s="7" t="n"/>
@@ -858,68 +814,69 @@
       <c r="G3" s="4" t="n"/>
       <c r="H3" s="5" t="n"/>
     </row>
-    <row r="4" ht="29.1" customHeight="1">
-      <c r="B4" s="28" t="inlineStr">
+    <row r="4" ht="29" customHeight="1">
+      <c r="B4" s="27" t="inlineStr">
         <is>
           <t>Configurações:</t>
         </is>
       </c>
-      <c r="C4" s="29" t="n"/>
-      <c r="D4" s="30" t="n"/>
-      <c r="F4" s="28" t="inlineStr">
+      <c r="C4" s="28" t="n"/>
+      <c r="D4" s="29" t="n"/>
+      <c r="F4" s="27" t="inlineStr">
         <is>
           <t>Instruções:</t>
         </is>
       </c>
-      <c r="G4" s="29" t="n"/>
-      <c r="H4" s="30" t="n"/>
-    </row>
-    <row r="5" ht="36.95" customHeight="1">
-      <c r="B5" s="31" t="inlineStr">
+      <c r="G4" s="28" t="n"/>
+      <c r="H4" s="29" t="n"/>
+    </row>
+    <row r="5" ht="48.75" customHeight="1">
+      <c r="B5" s="30" t="inlineStr">
         <is>
           <t>Apenas obter dados dos links cujos campos da linha estão vazios (mais seguro)</t>
         </is>
       </c>
-      <c r="C5" s="21" t="n"/>
-      <c r="D5" s="10" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F5" s="19" t="inlineStr">
+      <c r="C5" s="20" t="n"/>
+      <c r="D5" s="11" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F5" s="18" t="inlineStr">
         <is>
           <t xml:space="preserve">    1. Insira o novo link na primeira linha vazia da tabela, na coluna de "Links".
     2. Não se preocupe nem com o estilo, nem com os valores das células da nova linha. Tudo isso será arrumado pelo programa.
-    3. Vá para a linha de comando na pasta deste arquivo e execute "scrapy crawl linkedin". Caso haja erros, siga as instruções que aparecerem na tela.</t>
-        </is>
-      </c>
-      <c r="G5" s="20" t="n"/>
-      <c r="H5" s="21" t="n"/>
-    </row>
-    <row r="6" ht="45.95" customHeight="1">
-      <c r="B6" s="33" t="inlineStr">
-        <is>
-          <t>Tentar obter dados de páginas que foram marcadas como "Não é uma pessoa"</t>
-        </is>
-      </c>
-      <c r="C6" s="30" t="n"/>
-      <c r="D6" s="32" t="inlineStr">
+    3. Salve e feche o Excel.
+    4. Execute o programa "webcrawler.exe".</t>
+        </is>
+      </c>
+      <c r="G5" s="19" t="n"/>
+      <c r="H5" s="20" t="n"/>
+    </row>
+    <row r="6" ht="46" customHeight="1">
+      <c r="B6" s="32" t="inlineStr">
+        <is>
+          <t>Tentar obter dados de páginas que foram marcadas como "Não é uma pessoa" (ligue apenas se achar que há erros)</t>
+        </is>
+      </c>
+      <c r="C6" s="29" t="n"/>
+      <c r="D6" s="31" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="E6" s="12" t="n"/>
-      <c r="F6" s="22" t="n"/>
-      <c r="H6" s="24" t="n"/>
+      <c r="E6" s="10" t="n"/>
+      <c r="F6" s="21" t="n"/>
+      <c r="H6" s="23" t="n"/>
     </row>
     <row r="7" ht="39" customHeight="1">
-      <c r="D7" s="12" t="n"/>
-      <c r="E7" s="12" t="n"/>
-      <c r="F7" s="25" t="n"/>
-      <c r="G7" s="26" t="n"/>
-      <c r="H7" s="27" t="n"/>
-    </row>
-    <row r="9" ht="18.75" customHeight="1">
+      <c r="D7" s="10" t="n"/>
+      <c r="E7" s="10" t="n"/>
+      <c r="F7" s="24" t="n"/>
+      <c r="G7" s="25" t="n"/>
+      <c r="H7" s="26" t="n"/>
+    </row>
+    <row r="9" ht="20" customHeight="1">
       <c r="B9" s="8" t="inlineStr">
         <is>
           <t>Conta existe</t>
@@ -956,38 +913,38 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="315" customHeight="1">
-      <c r="B10" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C10" s="38" t="inlineStr">
+    <row r="10" ht="340" customHeight="1">
+      <c r="B10" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C10" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/rebecca-liu-93a12a28/</t>
         </is>
       </c>
-      <c r="D10" s="38" t="inlineStr">
+      <c r="D10" s="16" t="inlineStr">
         <is>
           <t>Rebecca</t>
         </is>
       </c>
-      <c r="E10" s="38" t="inlineStr">
+      <c r="E10" s="16" t="inlineStr">
         <is>
           <t>Liu</t>
         </is>
       </c>
-      <c r="F10" s="38" t="inlineStr">
+      <c r="F10" s="16" t="inlineStr">
         <is>
           <t>Senior Consultant at The Talent Company Ltd.</t>
         </is>
       </c>
-      <c r="G10" s="38" t="inlineStr">
+      <c r="G10" s="16" t="inlineStr">
         <is>
           <t>Toronto, Canada Area</t>
         </is>
       </c>
-      <c r="H10" s="38" t="inlineStr">
+      <c r="H10" s="16" t="inlineStr">
         <is>
           <t>The Talent Company is an HR Solutions Firm. We work closely with our clients to FIND, KEEP, REWARD and TRANSITION their talent. 
 With offices in Toronto, Mississauga and Markham, we support our clients in building, developing and retaining a highly engaged, high-performing workforce that is focused on achieving their business strategies and goals.
@@ -1001,369 +958,369 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="31.5" customHeight="1">
-      <c r="B11" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C11" s="36" t="inlineStr">
+    <row r="11" ht="34" customHeight="1">
+      <c r="B11" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C11" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/ed-woodward-7ba2b968</t>
         </is>
       </c>
-      <c r="D11" s="38" t="inlineStr">
+      <c r="D11" s="16" t="inlineStr">
         <is>
           <t>Ed</t>
         </is>
       </c>
-      <c r="E11" s="38" t="inlineStr">
+      <c r="E11" s="16" t="inlineStr">
         <is>
           <t>Woodward</t>
         </is>
       </c>
-      <c r="F11" s="38" t="inlineStr">
+      <c r="F11" s="16" t="inlineStr">
         <is>
           <t>General Manager at Northstar CG, LP.</t>
         </is>
       </c>
-      <c r="G11" s="38" t="inlineStr">
+      <c r="G11" s="16" t="inlineStr">
         <is>
           <t>La Center, Washington</t>
         </is>
       </c>
-      <c r="H11" s="38" t="inlineStr">
+      <c r="H11" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="126" customHeight="1">
-      <c r="B12" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C12" s="36" t="inlineStr">
+    <row r="12" ht="136" customHeight="1">
+      <c r="B12" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C12" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/neil-bath-76621045</t>
         </is>
       </c>
-      <c r="D12" s="38" t="inlineStr">
+      <c r="D12" s="16" t="inlineStr">
         <is>
           <t>Neil</t>
         </is>
       </c>
-      <c r="E12" s="38" t="inlineStr">
+      <c r="E12" s="16" t="inlineStr">
         <is>
           <t>Bath</t>
         </is>
       </c>
-      <c r="F12" s="38" t="inlineStr">
+      <c r="F12" s="16" t="inlineStr">
         <is>
           <t>Marine insurance broker</t>
         </is>
       </c>
-      <c r="G12" s="38" t="inlineStr">
+      <c r="G12" s="16" t="inlineStr">
         <is>
           <t>Miami, Florida</t>
         </is>
       </c>
-      <c r="H12" s="38" t="inlineStr">
+      <c r="H12" s="16" t="inlineStr">
         <is>
           <t>Many years of experience in all aspects of Marine Insurance &amp; Reinsurance, including business development, client servicing, placing of business and handling of claims. Specializing primarily in Hull &amp; Machinery, Protection &amp; Indemnity, Charterers Liabilities, Port &amp; Terminal Operators, Marine Cargo including STP's, with particular emphasis on Latin America.</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="157.5" customHeight="1">
-      <c r="B13" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C13" s="36" t="inlineStr">
+    <row r="13" ht="170" customHeight="1">
+      <c r="B13" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C13" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jim-cassell-171918b8</t>
         </is>
       </c>
-      <c r="D13" s="38" t="inlineStr">
+      <c r="D13" s="16" t="inlineStr">
         <is>
           <t>Jim</t>
         </is>
       </c>
-      <c r="E13" s="38" t="inlineStr">
+      <c r="E13" s="16" t="inlineStr">
         <is>
           <t>Cassell</t>
         </is>
       </c>
-      <c r="F13" s="38" t="inlineStr">
+      <c r="F13" s="16" t="inlineStr">
         <is>
           <t>GIS Engineering Technician at NiSource</t>
         </is>
       </c>
-      <c r="G13" s="38" t="inlineStr">
+      <c r="G13" s="16" t="inlineStr">
         <is>
           <t>Columbus, Ohio Area</t>
         </is>
       </c>
-      <c r="H13" s="38" t="inlineStr">
+      <c r="H13" s="16" t="inlineStr">
         <is>
           <t>As a professional in the field of business applications who also has a background in customer service, I have unique insight into both sides of business processes.  I have experience in determining requirements for process improvement projects, as well as testing and training during project implementation.  I also have extensive experience in the system administration side of applications support.  This experience has given me a big picture perspective on business processes.</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="23.25" customHeight="1">
-      <c r="B14" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C14" s="36" t="inlineStr">
+    <row r="14" ht="25" customHeight="1">
+      <c r="B14" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C14" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/claudio-silveira-888b741b0/</t>
         </is>
       </c>
-      <c r="D14" s="38" t="inlineStr">
+      <c r="D14" s="16" t="inlineStr">
         <is>
           <t>Claudio</t>
         </is>
       </c>
-      <c r="E14" s="38" t="inlineStr">
+      <c r="E14" s="16" t="inlineStr">
         <is>
           <t>Silveira</t>
         </is>
       </c>
-      <c r="F14" s="38" t="inlineStr">
+      <c r="F14" s="16" t="inlineStr">
         <is>
           <t>--</t>
         </is>
       </c>
-      <c r="G14" s="38" t="inlineStr">
+      <c r="G14" s="16" t="inlineStr">
         <is>
           <t>Brazil</t>
         </is>
       </c>
-      <c r="H14" s="38" t="inlineStr">
+      <c r="H14" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="157.5" customHeight="1">
-      <c r="B15" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C15" s="36" t="inlineStr">
+    <row r="15" ht="170" customHeight="1">
+      <c r="B15" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C15" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/boristai?trk=public_profile_browsemap_profile-result-card_result-card_full-click</t>
         </is>
       </c>
-      <c r="D15" s="38" t="inlineStr">
+      <c r="D15" s="16" t="inlineStr">
         <is>
           <t>Boris</t>
         </is>
       </c>
-      <c r="E15" s="38" t="inlineStr">
+      <c r="E15" s="16" t="inlineStr">
         <is>
           <t>Tai</t>
         </is>
       </c>
-      <c r="F15" s="38" t="inlineStr">
+      <c r="F15" s="16" t="inlineStr">
         <is>
           <t>Talent Acquisition Specialist at Loblaw Data Insight &amp; Analytics</t>
         </is>
       </c>
-      <c r="G15" s="38" t="inlineStr">
+      <c r="G15" s="16" t="inlineStr">
         <is>
           <t>Toronto, Canada Area</t>
         </is>
       </c>
-      <c r="H15" s="38" t="inlineStr">
+      <c r="H15" s="16" t="inlineStr">
         <is>
           <t>Experienced as a recruitment consultant providing recruiting services to banking and financial clients in the GTA area. Specializing in IT and business roles for both contract and full time positions. It is my goal to provide a smooth recruitment process for client and candidates, ensuring that the best possible talent is delivered in a quick and efficient manner.
 Specialties: Recruitment, Client Management, Human Resources</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="47.25" customHeight="1">
-      <c r="B16" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C16" s="36" t="inlineStr">
+    <row r="16" ht="51" customHeight="1">
+      <c r="B16" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C16" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/sammar-badawi?trk=public_profile_browsemap_profile-result-card_result-card_full-click</t>
         </is>
       </c>
-      <c r="D16" s="38" t="inlineStr">
+      <c r="D16" s="16" t="inlineStr">
         <is>
           <t>Sammar</t>
         </is>
       </c>
-      <c r="E16" s="38" t="inlineStr">
+      <c r="E16" s="16" t="inlineStr">
         <is>
           <t>Badawi</t>
         </is>
       </c>
-      <c r="F16" s="38" t="inlineStr">
+      <c r="F16" s="16" t="inlineStr">
         <is>
           <t>Talent Acquisition Partner at FreshBooks - We're Hiring!</t>
         </is>
       </c>
-      <c r="G16" s="38" t="inlineStr">
+      <c r="G16" s="16" t="inlineStr">
         <is>
           <t>Toronto, Ontario, Canada</t>
         </is>
       </c>
-      <c r="H16" s="38" t="inlineStr">
+      <c r="H16" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="47.25" customHeight="1">
-      <c r="B17" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C17" s="36" t="inlineStr">
+    <row r="17" ht="51" customHeight="1">
+      <c r="B17" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C17" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jessica-portelini-a09972161?trk=public_profile_browsemap_profile-result-card_result-card_full-click</t>
         </is>
       </c>
-      <c r="D17" s="38" t="inlineStr">
+      <c r="D17" s="16" t="inlineStr">
         <is>
           <t>Jessica</t>
         </is>
       </c>
-      <c r="E17" s="38" t="inlineStr">
+      <c r="E17" s="16" t="inlineStr">
         <is>
           <t>Portelini</t>
         </is>
       </c>
-      <c r="F17" s="38" t="inlineStr">
+      <c r="F17" s="16" t="inlineStr">
         <is>
           <t>Recruitment Manager at Apex Talent - We're Hiring Now!</t>
         </is>
       </c>
-      <c r="G17" s="38" t="inlineStr">
+      <c r="G17" s="16" t="inlineStr">
         <is>
           <t>Toronto, Canada Area</t>
         </is>
       </c>
-      <c r="H17" s="38" t="inlineStr">
+      <c r="H17" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="46.5" customHeight="1">
-      <c r="B18" s="37" t="inlineStr">
+    <row r="18" ht="50" customHeight="1">
+      <c r="B18" s="15" t="inlineStr">
         <is>
           <t>Não é uma pessoa</t>
         </is>
       </c>
-      <c r="C18" s="36" t="inlineStr">
+      <c r="C18" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jim-cassell-171918b7</t>
         </is>
       </c>
-      <c r="D18" s="38" t="n"/>
-      <c r="E18" s="38" t="n"/>
-      <c r="F18" s="38" t="n"/>
-      <c r="G18" s="38" t="n"/>
-      <c r="H18" s="38" t="n"/>
-    </row>
-    <row r="19" ht="46.5" customHeight="1">
-      <c r="B19" s="37" t="inlineStr">
+      <c r="D18" s="16" t="n"/>
+      <c r="E18" s="16" t="n"/>
+      <c r="F18" s="16" t="n"/>
+      <c r="G18" s="16" t="n"/>
+      <c r="H18" s="16" t="n"/>
+    </row>
+    <row r="19" ht="50" customHeight="1">
+      <c r="B19" s="15" t="inlineStr">
         <is>
           <t>Não é uma pessoa</t>
         </is>
       </c>
-      <c r="C19" s="36" t="inlineStr">
+      <c r="C19" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/company/mark/</t>
         </is>
       </c>
-      <c r="D19" s="38" t="n"/>
-      <c r="E19" s="38" t="n"/>
-      <c r="F19" s="38" t="n"/>
-      <c r="G19" s="38" t="n"/>
-      <c r="H19" s="38" t="n"/>
-    </row>
-    <row r="20" ht="141.75" customHeight="1">
-      <c r="B20" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C20" s="36" t="inlineStr">
+      <c r="D19" s="16" t="n"/>
+      <c r="E19" s="16" t="n"/>
+      <c r="F19" s="16" t="n"/>
+      <c r="G19" s="16" t="n"/>
+      <c r="H19" s="16" t="n"/>
+    </row>
+    <row r="20" ht="153" customHeight="1">
+      <c r="B20" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C20" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/kaelahrussell/</t>
         </is>
       </c>
-      <c r="D20" s="38" t="inlineStr">
+      <c r="D20" s="16" t="inlineStr">
         <is>
           <t>Kaelah</t>
         </is>
       </c>
-      <c r="E20" s="38" t="inlineStr">
+      <c r="E20" s="16" t="inlineStr">
         <is>
           <t>Russell</t>
         </is>
       </c>
-      <c r="F20" s="38" t="inlineStr">
+      <c r="F20" s="16" t="inlineStr">
         <is>
           <t>Senior Talent Acquisition Partner at Prodigy Game</t>
         </is>
       </c>
-      <c r="G20" s="38" t="inlineStr">
+      <c r="G20" s="16" t="inlineStr">
         <is>
           <t>Toronto, Ontario, Canada</t>
         </is>
       </c>
-      <c r="H20" s="38" t="inlineStr">
+      <c r="H20" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">We've all heard that saying 'do what you love, and love what you do'. Well, I'm happy to say that's exactly what I'm doing!  I've built a career in talent acquisition, starting in the agency world, then transitioned to corporate recruitment. I've become a trusted business partner and advisor when it comes to all things recruitment.  I love the excitement in finding the right person and helping Prodigy Game become stronger and better by adding top talent. </t>
         </is>
       </c>
     </row>
-    <row r="21" ht="189" customHeight="1">
-      <c r="B21" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C21" s="38" t="inlineStr">
+    <row r="21" ht="204" customHeight="1">
+      <c r="B21" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C21" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/bencrenca</t>
         </is>
       </c>
-      <c r="D21" s="38" t="inlineStr">
+      <c r="D21" s="16" t="inlineStr">
         <is>
           <t>Ben</t>
         </is>
       </c>
-      <c r="E21" s="38" t="inlineStr">
+      <c r="E21" s="16" t="inlineStr">
         <is>
           <t>Crenca</t>
         </is>
       </c>
-      <c r="F21" s="38" t="inlineStr">
+      <c r="F21" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">Talent Acquisition | Employer Branding | Building Culture </t>
         </is>
       </c>
-      <c r="G21" s="38" t="inlineStr">
+      <c r="G21" s="16" t="inlineStr">
         <is>
           <t>Washington D.C. Metro Area</t>
         </is>
       </c>
-      <c r="H21" s="38" t="inlineStr">
+      <c r="H21" s="16" t="inlineStr">
         <is>
           <t>WE ARE HIRING!
 Currently Seeking: 
@@ -1374,37 +1331,37 @@
       </c>
     </row>
     <row r="22" ht="409.5" customHeight="1">
-      <c r="B22" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C22" s="38" t="inlineStr">
+      <c r="B22" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C22" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/mandyj</t>
         </is>
       </c>
-      <c r="D22" s="38" t="inlineStr">
+      <c r="D22" s="16" t="inlineStr">
         <is>
           <t>Mandy</t>
         </is>
       </c>
-      <c r="E22" s="38" t="inlineStr">
+      <c r="E22" s="16" t="inlineStr">
         <is>
           <t>Jenkins</t>
         </is>
       </c>
-      <c r="F22" s="38" t="inlineStr">
+      <c r="F22" s="16" t="inlineStr">
         <is>
           <t>General Manager, The Compass Experiment at McClatchy</t>
         </is>
       </c>
-      <c r="G22" s="38" t="inlineStr">
+      <c r="G22" s="16" t="inlineStr">
         <is>
           <t>New York, New York</t>
         </is>
       </c>
-      <c r="H22" s="38" t="inlineStr">
+      <c r="H22" s="16" t="inlineStr">
         <is>
           <t>I started in digital journalism at a time when most jobs didn’t yet have titles, there were just tasks to be done and few people with the skills to do them. Now, after more than 16 years of working in newsrooms spanning newspapers, radio, television, service providers and digital startups, I am currently taking time out of the industry to be a fellow in the 2018-19 fellowship class of the John S. Knight fellowship at Stanford, where I will focus my research on disinformation and user experience. I am also currently the president of the Online News Association, the world's largest organization for digital journalists and media innovators. 
 I was most recently the Editor in Chief at Storyful, the leading social news and insights agency. I managed a team of 60+ social journalists who worked with the world's top newsrooms in surfacing, verifying and acquiring eyewitness journalism and debunking disinformation.  
@@ -1414,37 +1371,37 @@
       </c>
     </row>
     <row r="23" ht="409.5" customHeight="1">
-      <c r="B23" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C23" s="38" t="inlineStr">
+      <c r="B23" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C23" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/neilkane</t>
         </is>
       </c>
-      <c r="D23" s="38" t="inlineStr">
+      <c r="D23" s="16" t="inlineStr">
         <is>
           <t>Neil</t>
         </is>
       </c>
-      <c r="E23" s="38" t="inlineStr">
+      <c r="E23" s="16" t="inlineStr">
         <is>
           <t>Kane</t>
         </is>
       </c>
-      <c r="F23" s="38" t="inlineStr">
+      <c r="F23" s="16" t="inlineStr">
         <is>
           <t>Executive | Entrepreneur | Educator | Startup CEO  Author "The Innovator's Secret Formula"</t>
         </is>
       </c>
-      <c r="G23" s="38" t="inlineStr">
+      <c r="G23" s="16" t="inlineStr">
         <is>
           <t>Greater Detroit Area</t>
         </is>
       </c>
-      <c r="H23" s="38" t="inlineStr">
+      <c r="H23" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">"I've never been qualified for any job that I've had, but I always achieved success."​
 *  Entrepreneur/executive/innovator with 25 years of general management, sales, marketing and investment experience in environments ranging from nanotechnology to advanced materials to consumer products. 
@@ -1477,112 +1434,112 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="31.5" customHeight="1">
-      <c r="B24" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C24" s="38" t="inlineStr">
+    <row r="24" ht="34" customHeight="1">
+      <c r="B24" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C24" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/dixonheath</t>
         </is>
       </c>
-      <c r="D24" s="38" t="inlineStr">
+      <c r="D24" s="16" t="inlineStr">
         <is>
           <t>Heath</t>
         </is>
       </c>
-      <c r="E24" s="38" t="inlineStr">
+      <c r="E24" s="16" t="inlineStr">
         <is>
           <t>Dixon</t>
         </is>
       </c>
-      <c r="F24" s="38" t="inlineStr">
+      <c r="F24" s="16" t="inlineStr">
         <is>
           <t>Technology Lawyer at Amazon</t>
         </is>
       </c>
-      <c r="G24" s="38" t="inlineStr">
+      <c r="G24" s="16" t="inlineStr">
         <is>
           <t>Greater Seattle Area</t>
         </is>
       </c>
-      <c r="H24" s="38" t="inlineStr">
+      <c r="H24" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">Want to join the Amazon Legal Team?  Want to change the Internet?  </t>
         </is>
       </c>
     </row>
-    <row r="25" ht="173.25" customHeight="1">
-      <c r="B25" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C25" s="38" t="inlineStr">
+    <row r="25" ht="204" customHeight="1">
+      <c r="B25" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C25" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/erineriksson</t>
         </is>
       </c>
-      <c r="D25" s="38" t="inlineStr">
+      <c r="D25" s="16" t="inlineStr">
         <is>
           <t>Erin Elise</t>
         </is>
       </c>
-      <c r="E25" s="38" t="inlineStr">
+      <c r="E25" s="16" t="inlineStr">
         <is>
           <t>Eriksson</t>
         </is>
       </c>
-      <c r="F25" s="38" t="inlineStr">
+      <c r="F25" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">Social Impact, Global Health, &amp; Philanthropy Consultant </t>
         </is>
       </c>
-      <c r="G25" s="38" t="inlineStr">
+      <c r="G25" s="16" t="inlineStr">
         <is>
           <t>New York, New York</t>
         </is>
       </c>
-      <c r="H25" s="38" t="inlineStr">
+      <c r="H25" s="16" t="inlineStr">
         <is>
           <t>Experienced CSR professional and funder working with private sector, government, foundations, nonprofits, and bilateral/multilateral funders to improve global health outcomes. Success developing new strategic initiatives and enhancing brand visibility. Experience overseeing finances, budgeting, operations, and audit process for corporate foundation. Focus on corporate citizenship/corporate social responsibility, philanthropy, HIV/AIDS, monitoring &amp; evaluation, maternal health, key populations, social drivers, and employee engagement.</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="141.75" customHeight="1">
-      <c r="B26" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C26" s="38" t="inlineStr">
+    <row r="26" ht="187" customHeight="1">
+      <c r="B26" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C26" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/crystalhuang89</t>
         </is>
       </c>
-      <c r="D26" s="38" t="inlineStr">
+      <c r="D26" s="16" t="inlineStr">
         <is>
           <t>Crystal</t>
         </is>
       </c>
-      <c r="E26" s="38" t="inlineStr">
+      <c r="E26" s="16" t="inlineStr">
         <is>
           <t>Huang</t>
         </is>
       </c>
-      <c r="F26" s="38" t="inlineStr">
+      <c r="F26" s="16" t="inlineStr">
         <is>
           <t>Principal at New Enterprise Associates (NEA)</t>
         </is>
       </c>
-      <c r="G26" s="38" t="inlineStr">
+      <c r="G26" s="16" t="inlineStr">
         <is>
           <t>New York, New York</t>
         </is>
       </c>
-      <c r="H26" s="38" t="inlineStr">
+      <c r="H26" s="16" t="inlineStr">
         <is>
           <t>Venture capitalist at New Enterprise Associates (NEA) in New York, covering enterprise technologies (SaaS, infrastructure, security) and consumer internet. 
 Previously I was at GGV Capital in Silicon Valley where I worked closely with companies including Aptible, BigCommerce, BitSight, BrightWheel, HashiCorp, Headspin, MileZero, NS1, OpenDoor, Restless Bandit, Slack, Tile, Tray.io, Unravel Data and Wish.</t>
@@ -1590,37 +1547,37 @@
       </c>
     </row>
     <row r="27" ht="409.5" customHeight="1">
-      <c r="B27" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C27" s="38" t="inlineStr">
+      <c r="B27" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C27" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jasonhengels</t>
         </is>
       </c>
-      <c r="D27" s="38" t="inlineStr">
+      <c r="D27" s="16" t="inlineStr">
         <is>
           <t>Jason</t>
         </is>
       </c>
-      <c r="E27" s="38" t="inlineStr">
+      <c r="E27" s="16" t="inlineStr">
         <is>
           <t>Hengels</t>
         </is>
       </c>
-      <c r="F27" s="38" t="inlineStr">
+      <c r="F27" s="16" t="inlineStr">
         <is>
           <t>Founder, Exposure Security</t>
         </is>
       </c>
-      <c r="G27" s="38" t="inlineStr">
+      <c r="G27" s="16" t="inlineStr">
         <is>
           <t>Redwood City, California</t>
         </is>
       </c>
-      <c r="H27" s="38" t="inlineStr">
+      <c r="H27" s="16" t="inlineStr">
         <is>
           <t>Jason Hengels is a security executive with a broad range of skills who leads by example and creates an environment of excellence. He currently provides CISO-for-hire services to high profile companies, including industry names in the payment, insurance, multimedia and mortgage verticals. 
 Jason has worked through some of the most difficult situations in the security world, including APT breaches and remediation work, extortion attempts and DDoS attacks. He has led companies through PCI, SOC 2 and other compliance efforts and has presented at large conferences such as RSA. Beginning in 2014, Jason helped develop and refine the Information Security curriculum at Merritt College. Prior to founding Exposure Security, Jason built the Information Security programs at companies such as Box and CyberSource and held a senior-level position at Visa.
@@ -1629,223 +1586,223 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="47.25" customHeight="1">
-      <c r="B28" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C28" s="38" t="inlineStr">
+    <row r="28" ht="51" customHeight="1">
+      <c r="B28" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C28" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/ginamartinez13</t>
         </is>
       </c>
-      <c r="D28" s="38" t="inlineStr">
+      <c r="D28" s="16" t="inlineStr">
         <is>
           <t>Gina</t>
         </is>
       </c>
-      <c r="E28" s="38" t="inlineStr">
+      <c r="E28" s="16" t="inlineStr">
         <is>
           <t>Martinez</t>
         </is>
       </c>
-      <c r="F28" s="38" t="inlineStr">
+      <c r="F28" s="16" t="inlineStr">
         <is>
           <t>Breaking News Reporter</t>
         </is>
       </c>
-      <c r="G28" s="38" t="inlineStr">
+      <c r="G28" s="16" t="inlineStr">
         <is>
           <t>Brooklyn, New York</t>
         </is>
       </c>
-      <c r="H28" s="38" t="inlineStr">
+      <c r="H28" s="16" t="inlineStr">
         <is>
           <t>Experienced breaking news reporter with knowledge of social media, great interviewing skills and talent for news gathering in a busy news room.</t>
         </is>
       </c>
     </row>
-    <row r="29" ht="23.25" customHeight="1">
-      <c r="B29" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C29" s="38" t="inlineStr">
+    <row r="29" ht="25" customHeight="1">
+      <c r="B29" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C29" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/noobjun</t>
         </is>
       </c>
-      <c r="D29" s="38" t="inlineStr">
+      <c r="D29" s="16" t="inlineStr">
         <is>
           <t>Jun</t>
         </is>
       </c>
-      <c r="E29" s="38" t="inlineStr">
+      <c r="E29" s="16" t="inlineStr">
         <is>
           <t>Zhou</t>
         </is>
       </c>
-      <c r="F29" s="38" t="inlineStr">
+      <c r="F29" s="16" t="inlineStr">
         <is>
           <t>Software Engineer</t>
         </is>
       </c>
-      <c r="G29" s="38" t="inlineStr">
+      <c r="G29" s="16" t="inlineStr">
         <is>
           <t>Mountain View, California</t>
         </is>
       </c>
-      <c r="H29" s="38" t="inlineStr">
+      <c r="H29" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="31.5" customHeight="1">
-      <c r="B30" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C30" s="38" t="inlineStr">
+    <row r="30" ht="34" customHeight="1">
+      <c r="B30" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C30" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/priyabhardwaj</t>
         </is>
       </c>
-      <c r="D30" s="38" t="inlineStr">
+      <c r="D30" s="16" t="inlineStr">
         <is>
           <t>Priya</t>
         </is>
       </c>
-      <c r="E30" s="38" t="inlineStr">
+      <c r="E30" s="16" t="inlineStr">
         <is>
           <t>Bhardwaj</t>
         </is>
       </c>
-      <c r="F30" s="38" t="inlineStr">
+      <c r="F30" s="16" t="inlineStr">
         <is>
           <t>Vice President at JPMorgan Chase</t>
         </is>
       </c>
-      <c r="G30" s="38" t="inlineStr">
+      <c r="G30" s="16" t="inlineStr">
         <is>
           <t>Greater New York City Area</t>
         </is>
       </c>
-      <c r="H30" s="38" t="inlineStr">
+      <c r="H30" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="31" ht="47.25" customHeight="1">
-      <c r="B31" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C31" s="38" t="inlineStr">
+    <row r="31" ht="51" customHeight="1">
+      <c r="B31" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C31" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/mattniksch</t>
         </is>
       </c>
-      <c r="D31" s="38" t="inlineStr">
+      <c r="D31" s="16" t="inlineStr">
         <is>
           <t>Matt</t>
         </is>
       </c>
-      <c r="E31" s="38" t="inlineStr">
+      <c r="E31" s="16" t="inlineStr">
         <is>
           <t>Niksch</t>
         </is>
       </c>
-      <c r="F31" s="38" t="inlineStr">
+      <c r="F31" s="16" t="inlineStr">
         <is>
           <t>President at Noble Network of Charter Schools</t>
         </is>
       </c>
-      <c r="G31" s="38" t="inlineStr">
+      <c r="G31" s="16" t="inlineStr">
         <is>
           <t>Greater Chicago Area</t>
         </is>
       </c>
-      <c r="H31" s="38" t="inlineStr">
+      <c r="H31" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="204.75" customHeight="1">
-      <c r="B32" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C32" s="38" t="inlineStr">
+    <row r="32" ht="238" customHeight="1">
+      <c r="B32" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C32" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/iw3dlyw7</t>
         </is>
       </c>
-      <c r="D32" s="38" t="inlineStr">
+      <c r="D32" s="16" t="inlineStr">
         <is>
           <t>Jason</t>
         </is>
       </c>
-      <c r="E32" s="38" t="inlineStr">
+      <c r="E32" s="16" t="inlineStr">
         <is>
           <t>Child</t>
         </is>
       </c>
-      <c r="F32" s="38" t="inlineStr">
+      <c r="F32" s="16" t="inlineStr">
         <is>
           <t>CFO at Splunk</t>
         </is>
       </c>
-      <c r="G32" s="38" t="inlineStr">
+      <c r="G32" s="16" t="inlineStr">
         <is>
           <t>San Francisco Bay Area</t>
         </is>
       </c>
-      <c r="H32" s="38" t="inlineStr">
+      <c r="H32" s="16" t="inlineStr">
         <is>
           <t>Over 28 years of progressive experience in all aspects of Finance &amp; Strategy, Accounting, Capital Markets and Treasury. Specialize in scaling disruptive companies and working with/learning/gaining insight from awesome people.  Finance Director/VP during Amazon.com's growth from $900M sales run-rate in early 1999, to $50B+ run-rate in late 2010.  CFO during Groupon's growth from $750M in sales in 2010 to $7.6B in 2014.  CFO during Opendoor's growth from $400M in run-rate sales in early 2017 to $4B in early 2019.  Now, CFO during Splunk's transformation from on-prem to Cloud/Saas, while maintaining 40%+ annualized growth on our path to $5B in Revenue.</t>
         </is>
       </c>
     </row>
     <row r="33" ht="409.5" customHeight="1">
-      <c r="B33" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C33" s="38" t="inlineStr">
+      <c r="B33" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C33" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/billprater</t>
         </is>
       </c>
-      <c r="D33" s="38" t="inlineStr">
+      <c r="D33" s="16" t="inlineStr">
         <is>
           <t>Bill</t>
         </is>
       </c>
-      <c r="E33" s="38" t="inlineStr">
+      <c r="E33" s="16" t="inlineStr">
         <is>
           <t>Prater</t>
         </is>
       </c>
-      <c r="F33" s="38" t="inlineStr">
+      <c r="F33" s="16" t="inlineStr">
         <is>
           <t>Founder &amp; CEO | Mastermind Groups + Coaching + Team Building + Online Courses | Author – “How To Dominate Your Market”</t>
         </is>
       </c>
-      <c r="G33" s="38" t="inlineStr">
+      <c r="G33" s="16" t="inlineStr">
         <is>
           <t>Greater Seattle Area</t>
         </is>
       </c>
-      <c r="H33" s="38" t="inlineStr">
+      <c r="H33" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">WHAT I DO: Since 1999 I’ve helped Business Owners and Entrepreneurs in more than 50 different industries achieve real, measurable results using my unique approaches to grow revenue, increase cash flow and magnify business value.
 HOW I DO IT. I do this by incorporating several proprietary tools and techniques into the culture of the company and by empowering the team to manage the business. This consistently means the business owner’s personal efforts decline dramatically. 
@@ -1862,37 +1819,37 @@
       </c>
     </row>
     <row r="34" ht="409.5" customHeight="1">
-      <c r="B34" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C34" s="38" t="inlineStr">
+      <c r="B34" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C34" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/michaelarone</t>
         </is>
       </c>
-      <c r="D34" s="38" t="inlineStr">
+      <c r="D34" s="16" t="inlineStr">
         <is>
           <t>Michael</t>
         </is>
       </c>
-      <c r="E34" s="38" t="inlineStr">
+      <c r="E34" s="16" t="inlineStr">
         <is>
           <t>Arone</t>
         </is>
       </c>
-      <c r="F34" s="38" t="inlineStr">
+      <c r="F34" s="16" t="inlineStr">
         <is>
           <t>Chief Investment Strategist, Managing Director at State Street Global Advisors</t>
         </is>
       </c>
-      <c r="G34" s="38" t="inlineStr">
+      <c r="G34" s="16" t="inlineStr">
         <is>
           <t>Boston, Massachusetts</t>
         </is>
       </c>
-      <c r="H34" s="38" t="inlineStr">
+      <c r="H34" s="16" t="inlineStr">
         <is>
           <t>As a Managing Director of State Street Global Advisors and the Chief Investment Strategist for the US SPDR Business, I am responsible for expanding SSGA's footprint and thought leadership effort through frequent contributions to the financial news media, speaking engagements and client interactions. I am a frequent speaker at industry conferences and have authored several articles related to investment management practices. Here at SSGA I have previously served as the Global and EMEA Head of Portfolio Strategy as well as a senior portfolio manager in the Global Active Quantitative Equity Group.
 During my 20+-year career as a client-facing Investment Professional, I have served all major client segments, multiple asset classes and investment disciplines to help clients meet their long-term financial goals. I have substantial experience developing long-only and long-short quantitative strategies and managing investment portfolios using quantitative disciplines.
@@ -1901,38 +1858,38 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="189" customHeight="1">
-      <c r="B35" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C35" s="38" t="inlineStr">
+    <row r="35" ht="204" customHeight="1">
+      <c r="B35" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C35" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/srirampanyam</t>
         </is>
       </c>
-      <c r="D35" s="38" t="inlineStr">
+      <c r="D35" s="16" t="inlineStr">
         <is>
           <t>Sriram (Sri)</t>
         </is>
       </c>
-      <c r="E35" s="38" t="inlineStr">
+      <c r="E35" s="16" t="inlineStr">
         <is>
           <t>Panyam</t>
         </is>
       </c>
-      <c r="F35" s="38" t="inlineStr">
+      <c r="F35" s="16" t="inlineStr">
         <is>
           <t>Manager, Software Engineering at LinkedIn</t>
         </is>
       </c>
-      <c r="G35" s="38" t="inlineStr">
+      <c r="G35" s="16" t="inlineStr">
         <is>
           <t>Sunnyvale, California</t>
         </is>
       </c>
-      <c r="H35" s="38" t="inlineStr">
+      <c r="H35" s="16" t="inlineStr">
         <is>
           <t>I am passionate about building software and tools that power modern platforms and applications.  Over 15 years experience in wide ranging areas from embedded systems to gaming to mobile platforms to distributed systems and engineering leadership helps in understanding problems from various viewpoints and coming up with solutions (and sometimes problems) that are well thought out and impactful.
 Interests and Expertise: Scalable distributed systems, Service oriented architectures, Web services, API development and management, Language design.</t>
@@ -1940,37 +1897,37 @@
       </c>
     </row>
     <row r="36" ht="409.5" customHeight="1">
-      <c r="B36" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C36" s="38" t="inlineStr">
+      <c r="B36" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C36" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/dawsondavenport</t>
         </is>
       </c>
-      <c r="D36" s="38" t="inlineStr">
+      <c r="D36" s="16" t="inlineStr">
         <is>
           <t>Dawson</t>
         </is>
       </c>
-      <c r="E36" s="38" t="inlineStr">
+      <c r="E36" s="16" t="inlineStr">
         <is>
           <t>Davenport</t>
         </is>
       </c>
-      <c r="F36" s="38" t="inlineStr">
+      <c r="F36" s="16" t="inlineStr">
         <is>
           <t>President at TGG Realty</t>
         </is>
       </c>
-      <c r="G36" s="38" t="inlineStr">
+      <c r="G36" s="16" t="inlineStr">
         <is>
           <t>Costa Mesa, California</t>
         </is>
       </c>
-      <c r="H36" s="38" t="inlineStr">
+      <c r="H36" s="16" t="inlineStr">
         <is>
           <t>Dawson Davenport is an industry professional in business advisory and real estate services with over 35 years of experience encompassing REO/Receiver/Bankruptcy Assets, Real Estate Investments. Business Consulting, Business Operations,  Real Estate operations, Property Acquisition/Disposition, Property Renovation/Rehabilitation, and Asset Management.
 Mr. Davenport served as a key officer including President and Director of several real estate, real estate consulting and business consulting firms in Southern California.
@@ -1979,262 +1936,262 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="110.25" customHeight="1">
-      <c r="B37" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C37" s="38" t="inlineStr">
+    <row r="37" ht="119" customHeight="1">
+      <c r="B37" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C37" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/cameronpbean</t>
         </is>
       </c>
-      <c r="D37" s="38" t="inlineStr">
+      <c r="D37" s="16" t="inlineStr">
         <is>
           <t>Cameron</t>
         </is>
       </c>
-      <c r="E37" s="38" t="inlineStr">
+      <c r="E37" s="16" t="inlineStr">
         <is>
           <t>Bean</t>
         </is>
       </c>
-      <c r="F37" s="38" t="inlineStr">
+      <c r="F37" s="16" t="inlineStr">
         <is>
           <t>Assistant Vice President for Development &amp; Stewardship at Columbus State University</t>
         </is>
       </c>
-      <c r="G37" s="38" t="inlineStr">
+      <c r="G37" s="16" t="inlineStr">
         <is>
           <t>Columbus, Georgia</t>
         </is>
       </c>
-      <c r="H37" s="38" t="inlineStr">
+      <c r="H37" s="16" t="inlineStr">
         <is>
           <t>Certified Fund Raising Executive with successful track record in lean, fast-paced non-profit and educational organizations. Expertise includes annual and capital fundraising campaigns, corporate and foundation relations, stewardship programs, public relations, creative solutions, board development and consensus building.</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="31.5" customHeight="1">
-      <c r="B38" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C38" s="38" t="inlineStr">
+    <row r="38" ht="34" customHeight="1">
+      <c r="B38" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C38" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/weiguo1</t>
         </is>
       </c>
-      <c r="D38" s="38" t="inlineStr">
+      <c r="D38" s="16" t="inlineStr">
         <is>
           <t>Wei</t>
         </is>
       </c>
-      <c r="E38" s="38" t="inlineStr">
+      <c r="E38" s="16" t="inlineStr">
         <is>
           <t>Guo</t>
         </is>
       </c>
-      <c r="F38" s="38" t="inlineStr">
+      <c r="F38" s="16" t="inlineStr">
         <is>
           <t>Analyst at Whale Rock Capital Management LLC</t>
         </is>
       </c>
-      <c r="G38" s="38" t="inlineStr">
+      <c r="G38" s="16" t="inlineStr">
         <is>
           <t>Boston, Massachusetts</t>
         </is>
       </c>
-      <c r="H38" s="38" t="inlineStr">
+      <c r="H38" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="141.75" customHeight="1">
-      <c r="B39" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C39" s="38" t="inlineStr">
+    <row r="39" ht="153" customHeight="1">
+      <c r="B39" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C39" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jameskenly</t>
         </is>
       </c>
-      <c r="D39" s="38" t="inlineStr">
+      <c r="D39" s="16" t="inlineStr">
         <is>
           <t>James</t>
         </is>
       </c>
-      <c r="E39" s="38" t="inlineStr">
+      <c r="E39" s="16" t="inlineStr">
         <is>
           <t>Kenly</t>
         </is>
       </c>
-      <c r="F39" s="38" t="inlineStr">
+      <c r="F39" s="16" t="inlineStr">
         <is>
           <t>Cultivating community at 8150'</t>
         </is>
       </c>
-      <c r="G39" s="38" t="inlineStr">
+      <c r="G39" s="16" t="inlineStr">
         <is>
           <t>Avon, Colorado</t>
         </is>
       </c>
-      <c r="H39" s="38" t="inlineStr">
+      <c r="H39" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">Self-actualizing business leader with a passion for the mountains, business administration and community development. A Lean and creative systems thinker thriving at the intersection of what is and what is possible. Dedicated to facilitating the connection between people and purpose through integrated business systems that reinforce a compelling brand promise.
 </t>
         </is>
       </c>
     </row>
-    <row r="40" ht="157.5" customHeight="1">
-      <c r="B40" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C40" s="38" t="inlineStr">
+    <row r="40" ht="187" customHeight="1">
+      <c r="B40" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C40" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/joshrubinca</t>
         </is>
       </c>
-      <c r="D40" s="38" t="inlineStr">
+      <c r="D40" s="16" t="inlineStr">
         <is>
           <t>Josh</t>
         </is>
       </c>
-      <c r="E40" s="38" t="inlineStr">
+      <c r="E40" s="16" t="inlineStr">
         <is>
           <t>Rubin</t>
         </is>
       </c>
-      <c r="F40" s="38" t="inlineStr">
+      <c r="F40" s="16" t="inlineStr">
         <is>
           <t>Ask me how you can meet your 2020 business goals through strategic marketing!</t>
         </is>
       </c>
-      <c r="G40" s="38" t="inlineStr">
+      <c r="G40" s="16" t="inlineStr">
         <is>
           <t>Sacramento, California</t>
         </is>
       </c>
-      <c r="H40" s="38" t="inlineStr">
+      <c r="H40" s="16" t="inlineStr">
         <is>
           <t>I own Post Modern Marketing - a top digital marketing firm with locations in Sacramento, San Diego, Reno and Lexington. We were the region's 4th fastest growing company in 2018, 6th in 2019, and have been awarded as a top firm by several agencies.
 Specialties: Web development, SEO, web marketing, identity/brand development, process architect.  Using modern technology without losing focus on customer service and basic marketing principals.</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="141.75" customHeight="1">
-      <c r="B41" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C41" s="38" t="inlineStr">
+    <row r="41" ht="153" customHeight="1">
+      <c r="B41" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C41" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/brianbehlendorf</t>
         </is>
       </c>
-      <c r="D41" s="38" t="inlineStr">
+      <c r="D41" s="16" t="inlineStr">
         <is>
           <t>Brian</t>
         </is>
       </c>
-      <c r="E41" s="38" t="inlineStr">
+      <c r="E41" s="16" t="inlineStr">
         <is>
           <t>Behlendorf</t>
         </is>
       </c>
-      <c r="F41" s="38" t="inlineStr">
+      <c r="F41" s="16" t="inlineStr">
         <is>
           <t>Executive Director of the Hyperledger Project</t>
         </is>
       </c>
-      <c r="G41" s="38" t="inlineStr">
+      <c r="G41" s="16" t="inlineStr">
         <is>
           <t>San Francisco Bay Area</t>
         </is>
       </c>
-      <c r="H41" s="38" t="inlineStr">
+      <c r="H41" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">I've dedicated my career to connecting and empowering the Free Software and Open Source community to solve hard technology problems and have a positive societal impact.  I've done this wearing many different hats - as a startup company founder, as an advisor to the U.S. government, as a board member at various non-profits and consortia, as a YGL and employee of the World Economic Forum, and as an investor.  </t>
         </is>
       </c>
     </row>
-    <row r="42" ht="47.25" customHeight="1">
-      <c r="B42" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C42" s="38" t="inlineStr">
+    <row r="42" ht="51" customHeight="1">
+      <c r="B42" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C42" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/willjohnson</t>
         </is>
       </c>
-      <c r="D42" s="38" t="inlineStr">
+      <c r="D42" s="16" t="inlineStr">
         <is>
           <t>Will</t>
         </is>
       </c>
-      <c r="E42" s="38" t="inlineStr">
+      <c r="E42" s="16" t="inlineStr">
         <is>
           <t>Johnson</t>
         </is>
       </c>
-      <c r="F42" s="38" t="inlineStr">
+      <c r="F42" s="16" t="inlineStr">
         <is>
           <t>Director Of Software Engineering, Search at ServiceNow</t>
         </is>
       </c>
-      <c r="G42" s="38" t="inlineStr">
+      <c r="G42" s="16" t="inlineStr">
         <is>
           <t>Greater Boston Area</t>
         </is>
       </c>
-      <c r="H42" s="38" t="inlineStr">
+      <c r="H42" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
-    <row r="43" ht="173.25" customHeight="1">
-      <c r="B43" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C43" s="38" t="inlineStr">
+    <row r="43" ht="204" customHeight="1">
+      <c r="B43" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C43" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/petejadavies</t>
         </is>
       </c>
-      <c r="D43" s="38" t="inlineStr">
+      <c r="D43" s="16" t="inlineStr">
         <is>
           <t>Pete</t>
         </is>
       </c>
-      <c r="E43" s="38" t="inlineStr">
+      <c r="E43" s="16" t="inlineStr">
         <is>
           <t>Davies</t>
         </is>
       </c>
-      <c r="F43" s="38" t="inlineStr">
+      <c r="F43" s="16" t="inlineStr">
         <is>
           <t>Recovering journalist.</t>
         </is>
       </c>
-      <c r="G43" s="38" t="inlineStr">
+      <c r="G43" s="16" t="inlineStr">
         <is>
           <t>San Francisco Bay Area</t>
         </is>
       </c>
-      <c r="H43" s="38" t="inlineStr">
+      <c r="H43" s="16" t="inlineStr">
         <is>
           <t>I lead the Identity, Search, and Content teams at LinkedIn, where we are enabling our members to build and engage with communities that help them to become more productive and successful.
 Formerly... Product Lead and Product Scientist (Medium); Growth &amp; Analytics Lead and Product Lead (Automattic/WordPress.com); General Manager (TerraPass); Journalist &amp; Senior Producer (BBC Radio).
@@ -2242,76 +2199,76 @@
         </is>
       </c>
     </row>
-    <row r="44" ht="173.25" customHeight="1">
-      <c r="B44" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C44" s="38" t="inlineStr">
+    <row r="44" ht="50" customHeight="1">
+      <c r="B44" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C44" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/shyamnagarajan</t>
         </is>
       </c>
-      <c r="D44" s="38" t="inlineStr">
+      <c r="D44" s="16" t="inlineStr">
         <is>
           <t>Shyam</t>
         </is>
       </c>
-      <c r="E44" s="38" t="inlineStr">
+      <c r="E44" s="16" t="inlineStr">
         <is>
           <t>Nagarajan</t>
         </is>
       </c>
-      <c r="F44" s="38" t="inlineStr">
+      <c r="F44" s="16" t="inlineStr">
         <is>
           <t>Director, Go To Market Blockchain Networks at IBM Services</t>
         </is>
       </c>
-      <c r="G44" s="38" t="inlineStr">
+      <c r="G44" s="16" t="inlineStr">
         <is>
           <t>Greater New York City Area</t>
         </is>
       </c>
-      <c r="H44" s="38" t="inlineStr">
+      <c r="H44" s="16" t="inlineStr">
         <is>
           <t>Experienced business growth (sales and technology) executive with sharp acumen for achieving business results.  Creative, resourceful and strategic in pursuing new initiatives from concept to completion.  High performance team leader with proven track record in driving change and managing growth.
 software portfolio, software revenue, sales leader, sales professionals, process management, overachieved, application server, growth markets, high performance, sales management and execution</t>
         </is>
       </c>
     </row>
-    <row r="45" ht="236.25" customHeight="1">
-      <c r="B45" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C45" s="38" t="inlineStr">
+    <row r="45" ht="255" customHeight="1">
+      <c r="B45" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C45" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/leopmcguire</t>
         </is>
       </c>
-      <c r="D45" s="38" t="inlineStr">
+      <c r="D45" s="16" t="inlineStr">
         <is>
           <t>Leo P.</t>
         </is>
       </c>
-      <c r="E45" s="38" t="inlineStr">
+      <c r="E45" s="16" t="inlineStr">
         <is>
           <t>McGuire, MBA</t>
         </is>
       </c>
-      <c r="F45" s="38" t="inlineStr">
+      <c r="F45" s="16" t="inlineStr">
         <is>
           <t>Head of Security/Dir. of Risk Management</t>
         </is>
       </c>
-      <c r="G45" s="38" t="inlineStr">
+      <c r="G45" s="16" t="inlineStr">
         <is>
           <t>Paramus, New Jersey</t>
         </is>
       </c>
-      <c r="H45" s="38" t="inlineStr">
+      <c r="H45" s="16" t="inlineStr">
         <is>
           <t>An experienced chief executive who successfully led a large governmental organization ($58M/550 employees), that enhanced revenues and contained costs while developing innovative solutions to complex issues. 
 Solution-oriented leadership understanding the value of team building towards achieving strategic goals on behalf of the organization.
@@ -2319,75 +2276,75 @@
         </is>
       </c>
     </row>
-    <row r="46" ht="47.25" customHeight="1">
-      <c r="B46" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C46" s="36" t="inlineStr">
+    <row r="46" ht="51" customHeight="1">
+      <c r="B46" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C46" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/kristalane</t>
         </is>
       </c>
-      <c r="D46" s="38" t="inlineStr">
+      <c r="D46" s="16" t="inlineStr">
         <is>
           <t>Krista</t>
         </is>
       </c>
-      <c r="E46" s="38" t="inlineStr">
+      <c r="E46" s="16" t="inlineStr">
         <is>
           <t>Lane</t>
         </is>
       </c>
-      <c r="F46" s="38" t="inlineStr">
+      <c r="F46" s="16" t="inlineStr">
         <is>
           <t>Executive Producer of Special Projects at CBS4/FOX59</t>
         </is>
       </c>
-      <c r="G46" s="38" t="inlineStr">
+      <c r="G46" s="16" t="inlineStr">
         <is>
           <t>Indianapolis, Indiana</t>
         </is>
       </c>
-      <c r="H46" s="38" t="inlineStr">
+      <c r="H46" s="16" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
     </row>
     <row r="47" ht="409.5" customHeight="1">
-      <c r="B47" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C47" s="36" t="inlineStr">
+      <c r="B47" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C47" s="14" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/schmidtmaxr</t>
         </is>
       </c>
-      <c r="D47" s="38" t="inlineStr">
+      <c r="D47" s="16" t="inlineStr">
         <is>
           <t>Max</t>
         </is>
       </c>
-      <c r="E47" s="38" t="inlineStr">
+      <c r="E47" s="16" t="inlineStr">
         <is>
           <t>Schmidt</t>
         </is>
       </c>
-      <c r="F47" s="38" t="inlineStr">
+      <c r="F47" s="16" t="inlineStr">
         <is>
           <t>Chief Information Officer at The World</t>
         </is>
       </c>
-      <c r="G47" s="38" t="inlineStr">
+      <c r="G47" s="16" t="inlineStr">
         <is>
           <t>Miami/Fort Lauderdale Area</t>
         </is>
       </c>
-      <c r="H47" s="38" t="inlineStr">
+      <c r="H47" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Information technology and business leader with extensive travel and hospitality experience.  Adept at implementing innovative technology that breaks legacy barriers to enhance customer experience, reduce cost and improve operational efficiencies. Implements an engaging and culture-based leadership style with the proven ability to motivate and perform at high levels of productivity.  Proven track record with managing multi-million dollar budgets and driving millions of incremental revenue through the deployment of technology.  Experience in managing global IT operations consisting of over 26 shoreside corporate offices and 42 ships located in the USA, Latin America, Asia and Europe. 
@@ -2407,38 +2364,38 @@
         </is>
       </c>
     </row>
-    <row r="48" ht="220.5" customHeight="1">
-      <c r="B48" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C48" s="38" t="inlineStr">
+    <row r="48" ht="238" customHeight="1">
+      <c r="B48" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C48" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/nedstaebler</t>
         </is>
       </c>
-      <c r="D48" s="38" t="inlineStr">
+      <c r="D48" s="16" t="inlineStr">
         <is>
           <t>Ned</t>
         </is>
       </c>
-      <c r="E48" s="38" t="inlineStr">
+      <c r="E48" s="16" t="inlineStr">
         <is>
           <t>Staebler</t>
         </is>
       </c>
-      <c r="F48" s="38" t="inlineStr">
+      <c r="F48" s="16" t="inlineStr">
         <is>
           <t>Vice President for Economic Development at Wayne State University and President and CEO of TechTown</t>
         </is>
       </c>
-      <c r="G48" s="38" t="inlineStr">
+      <c r="G48" s="16" t="inlineStr">
         <is>
           <t>Ann Arbor, Michigan</t>
         </is>
       </c>
-      <c r="H48" s="38" t="inlineStr">
+      <c r="H48" s="16" t="inlineStr">
         <is>
           <t>Entrepreneurial leader experienced in crafting and implementing statewide innovation-based economic development policy and internationally recognized best practices in community-based inclusive economic development.
 Extensive experience building and leading successful teams of talented vice president and director level managers in both startup and Fortune 150 business settings. Far-reaching connections in the business community in Southeast Michigan and across the state. Proven track record of building consensus and strategic coalitions with local, statewide and regional economic development and industry groups.</t>
@@ -2446,37 +2403,37 @@
       </c>
     </row>
     <row r="49" ht="409.5" customHeight="1">
-      <c r="B49" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C49" s="38" t="inlineStr">
+      <c r="B49" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C49" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/donbora</t>
         </is>
       </c>
-      <c r="D49" s="38" t="inlineStr">
+      <c r="D49" s="16" t="inlineStr">
         <is>
           <t>Don</t>
         </is>
       </c>
-      <c r="E49" s="38" t="inlineStr">
+      <c r="E49" s="16" t="inlineStr">
         <is>
           <t>Bora</t>
         </is>
       </c>
-      <c r="F49" s="38" t="inlineStr">
+      <c r="F49" s="16" t="inlineStr">
         <is>
           <t>Co-Founder and Principal of Technology Eight Bit Studios. Public Speaker</t>
         </is>
       </c>
-      <c r="G49" s="38" t="inlineStr">
+      <c r="G49" s="16" t="inlineStr">
         <is>
           <t>Chicago, Illinois</t>
         </is>
       </c>
-      <c r="H49" s="38" t="inlineStr">
+      <c r="H49" s="16" t="inlineStr">
         <is>
           <t>**Recruiters**
 And I say this with all of the love in my heart: I am currently partner/principal in technology and co-founder of Eight Bit Studios where I help run the company and oversee all things tech. I am not leaving my current positions. Thank you for your interest insofar as reading this and good luck in your search. 
@@ -2503,37 +2460,37 @@
       </c>
     </row>
     <row r="50" ht="409.5" customHeight="1">
-      <c r="B50" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C50" s="38" t="inlineStr">
+      <c r="B50" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C50" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/lynndessert</t>
         </is>
       </c>
-      <c r="D50" s="38" t="inlineStr">
+      <c r="D50" s="16" t="inlineStr">
         <is>
           <t>Lynn</t>
         </is>
       </c>
-      <c r="E50" s="38" t="inlineStr">
+      <c r="E50" s="16" t="inlineStr">
         <is>
           <t>Dessert MBA, MCC</t>
         </is>
       </c>
-      <c r="F50" s="38" t="inlineStr">
+      <c r="F50" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">Master Certified Coach | Executive Leadership Coach | Mentor Coach | Past President ICF CAC | Speaker | 704-412-2852 </t>
         </is>
       </c>
-      <c r="G50" s="38" t="inlineStr">
+      <c r="G50" s="16" t="inlineStr">
         <is>
           <t>Charlotte, North Carolina Area</t>
         </is>
       </c>
-      <c r="H50" s="38" t="inlineStr">
+      <c r="H50" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">If I can be of service to your professional or personal development, contact me at 704-412-2852 or https://live.vcita.com/site/lynndessert.
 Executive Coaching
@@ -2560,75 +2517,75 @@
         </is>
       </c>
     </row>
-    <row r="51" ht="78.75" customHeight="1">
-      <c r="B51" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C51" s="38" t="inlineStr">
+    <row r="51" ht="85" customHeight="1">
+      <c r="B51" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C51" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/haileyhu</t>
         </is>
       </c>
-      <c r="D51" s="38" t="inlineStr">
+      <c r="D51" s="16" t="inlineStr">
         <is>
           <t>Hailey</t>
         </is>
       </c>
-      <c r="E51" s="38" t="inlineStr">
+      <c r="E51" s="16" t="inlineStr">
         <is>
           <t>Hu</t>
         </is>
       </c>
-      <c r="F51" s="38" t="inlineStr">
+      <c r="F51" s="16" t="inlineStr">
         <is>
           <t>Investment Director at AiiM Partners</t>
         </is>
       </c>
-      <c r="G51" s="38" t="inlineStr">
+      <c r="G51" s="16" t="inlineStr">
         <is>
           <t>San Francisco Bay Area</t>
         </is>
       </c>
-      <c r="H51" s="38" t="inlineStr">
+      <c r="H51" s="16" t="inlineStr">
         <is>
           <t>Investing in early-stage startups addressing climate change, sustainability, and access.  Experience in investing, strategy, operations, and business development globally. INSEAD MBA, Wharton undergrad, San Diego native.</t>
         </is>
       </c>
     </row>
-    <row r="52" ht="31.5" customHeight="1">
-      <c r="B52" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C52" s="38" t="inlineStr">
+    <row r="52" ht="34" customHeight="1">
+      <c r="B52" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C52" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/warald</t>
         </is>
       </c>
-      <c r="D52" s="38" t="inlineStr">
+      <c r="D52" s="16" t="inlineStr">
         <is>
           <t>Warald</t>
         </is>
       </c>
-      <c r="E52" s="38" t="inlineStr">
+      <c r="E52" s="16" t="inlineStr">
         <is>
           <t>一亩三分地</t>
         </is>
       </c>
-      <c r="F52" s="38" t="inlineStr">
+      <c r="F52" s="16" t="inlineStr">
         <is>
           <t>CEO at 1Point3Acres, LLC</t>
         </is>
       </c>
-      <c r="G52" s="38" t="inlineStr">
+      <c r="G52" s="16" t="inlineStr">
         <is>
           <t>Las Vegas, Nevada</t>
         </is>
       </c>
-      <c r="H52" s="38" t="inlineStr">
+      <c r="H52" s="16" t="inlineStr">
         <is>
           <t xml:space="preserve">一亩三分地伴你一起成长
 Together. Aim higher. Achieve more. </t>
@@ -2636,37 +2593,37 @@
       </c>
     </row>
     <row r="53" ht="409.5" customHeight="1">
-      <c r="B53" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C53" s="38" t="inlineStr">
+      <c r="B53" s="15" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C53" s="16" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/katiesowieja</t>
         </is>
       </c>
-      <c r="D53" s="38" t="inlineStr">
+      <c r="D53" s="16" t="inlineStr">
         <is>
           <t>Katie</t>
         </is>
       </c>
-      <c r="E53" s="38" t="inlineStr">
+      <c r="E53" s="16" t="inlineStr">
         <is>
           <t>Sowieja</t>
         </is>
       </c>
-      <c r="F53" s="38" t="inlineStr">
+      <c r="F53" s="16" t="inlineStr">
         <is>
           <t>Director of Brand Marketing</t>
         </is>
       </c>
-      <c r="G53" s="38" t="inlineStr">
+      <c r="G53" s="16" t="inlineStr">
         <is>
           <t>Greater Minneapolis-St. Paul Area</t>
         </is>
       </c>
-      <c r="H53" s="38" t="inlineStr">
+      <c r="H53" s="16" t="inlineStr">
         <is>
           <t>Delivering Growth Through Insight-Driven Strategy
 Accomplished marketing leader with both corporate and agency experience. Proven ability to develop insight-driven, innovative strategic marketing plans that facilitate business growth.
@@ -2677,101 +2634,7 @@
         </is>
       </c>
     </row>
-    <row r="54" ht="63" customHeight="1">
-      <c r="B54" s="37" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C54" s="36" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/rodrigo-miksian-magaldi</t>
-        </is>
-      </c>
-      <c r="D54" s="38" t="inlineStr">
-        <is>
-          <t>Rodrigo</t>
-        </is>
-      </c>
-      <c r="E54" s="38" t="inlineStr">
-        <is>
-          <t>Miksian Magaldi</t>
-        </is>
-      </c>
-      <c r="F54" s="38" t="inlineStr">
-        <is>
-          <t>Gerente de tecnologia na Poli Júnior</t>
-        </is>
-      </c>
-      <c r="G54" s="38" t="inlineStr">
-        <is>
-          <t>São Paulo, São Paulo, Brazil</t>
-        </is>
-      </c>
-      <c r="H54" s="38" t="inlineStr">
-        <is>
-          <t>Estudante do 7º semestre de Engenharia Elétrica (ênfase em computação) na Escola Politécnica da USP, e Gerente de Tecnologia da Poli Júnior. Desenvolvedor aficionado e apaixonado por dados.</t>
-        </is>
-      </c>
-    </row>
-    <row r="55" ht="63" customHeight="1">
-      <c r="B55" s="37" t="inlineStr">
-        <is>
-          <t>Sim (Cópia)</t>
-        </is>
-      </c>
-      <c r="C55" s="36" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/rodrigo-miksian-magaldi</t>
-        </is>
-      </c>
-      <c r="D55" s="38" t="inlineStr">
-        <is>
-          <t>Rodrigo</t>
-        </is>
-      </c>
-      <c r="E55" s="38" t="inlineStr">
-        <is>
-          <t>Miksian Magaldi</t>
-        </is>
-      </c>
-      <c r="F55" s="38" t="inlineStr">
-        <is>
-          <t>Gerente de tecnologia na Poli Júnior</t>
-        </is>
-      </c>
-      <c r="G55" s="38" t="inlineStr">
-        <is>
-          <t>São Paulo, São Paulo, Brazil</t>
-        </is>
-      </c>
-      <c r="H55" s="38" t="inlineStr">
-        <is>
-          <t>Estudante do 7º semestre de Engenharia Elétrica (ênfase em computação) na Escola Politécnica da USP, e Gerente de Tecnologia da Poli Júnior. Desenvolvedor aficionado e apaixonado por dados.</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" s="37" t="inlineStr">
-        <is>
-          <t>Não é uma pessoa</t>
-        </is>
-      </c>
-      <c r="C56" s="36" t="inlineStr">
-        <is>
-          <t>https://stackoverflow.com/questions/48030717/scrapy-404-error-http-status-code-is-not-handled-or-not-allowed</t>
-        </is>
-      </c>
-      <c r="D56" s="38" t="n"/>
-      <c r="E56" s="38" t="n"/>
-      <c r="F56" s="38" t="n"/>
-      <c r="G56" s="38" t="n"/>
-      <c r="H56" s="38" t="n"/>
-    </row>
-    <row r="57"/>
-    <row r="60">
-      <c r="H60" s="11" t="n"/>
-    </row>
+    <row r="54"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="F5:H7"/>
@@ -2782,175 +2645,51 @@
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D6">
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="0">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="0">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="1">
       <formula>"Sim"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4 B9:B1048576">
-    <cfRule type="containsText" priority="2" operator="containsText" dxfId="10" text="Não">
-      <formula>NOT(ISERROR(SEARCH("Não",B4)))</formula>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>"Não é uma pessoa"</formula>
     </cfRule>
-    <cfRule type="containsText" priority="1" operator="containsText" dxfId="9" text="Sim">
-      <formula>NOT(ISERROR(SEARCH("Sim",B4)))</formula>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1">
+      <formula>"Sim"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="0">
+      <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId139"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId140"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId141"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId142"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId143"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId144"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId145"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId146"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId147"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId148"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId149"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C11" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C12" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C13" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C14" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C15" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C16" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C18" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C20" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -2960,26 +2699,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:G15"/>
+  <dimension ref="B2:G17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.875" defaultRowHeight="15.75" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col width="10.875" customWidth="1" style="1" min="1" max="1"/>
+    <col width="10.83203125" customWidth="1" style="1" min="1" max="1"/>
     <col width="38.5" customWidth="1" style="1" min="2" max="2"/>
-    <col width="25.625" customWidth="1" style="1" min="3" max="3"/>
-    <col width="14.625" customWidth="1" style="7" min="4" max="4"/>
-    <col width="10.875" customWidth="1" style="3" min="5" max="5"/>
+    <col width="25.6640625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="14.6640625" customWidth="1" style="7" min="4" max="4"/>
+    <col width="10.83203125" customWidth="1" style="3" min="5" max="5"/>
     <col width="13" customWidth="1" style="3" min="6" max="6"/>
-    <col width="64.875" customWidth="1" style="1" min="7" max="7"/>
-    <col width="10.875" customWidth="1" style="1" min="8" max="71"/>
-    <col width="10.875" customWidth="1" style="1" min="72" max="16384"/>
+    <col width="64.83203125" customWidth="1" style="1" min="7" max="7"/>
+    <col width="10.83203125" customWidth="1" style="1" min="8" max="67"/>
+    <col width="10.83203125" customWidth="1" style="1" min="68" max="16384"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" ht="17" customHeight="1">
       <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Email</t>
@@ -3012,366 +2751,426 @@
       </c>
     </row>
     <row r="3" ht="31.5" customHeight="1">
-      <c r="B3" s="38" t="inlineStr">
+      <c r="B3" s="16" t="inlineStr">
         <is>
           <t>leslie.brown.comm@gmail.com</t>
         </is>
       </c>
-      <c r="C3" s="38" t="inlineStr">
+      <c r="C3" s="16" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D3" s="38" t="n">
+      <c r="D3" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="E3" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F3" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G3" s="17" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="31.5" customHeight="1">
+      <c r="B4" s="16" t="inlineStr">
+        <is>
+          <t>asdrubal_dos_santos@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D4" s="16" t="n">
+        <v>49</v>
+      </c>
+      <c r="E4" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F4" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G4" s="17" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="31.5" customHeight="1">
+      <c r="B5" s="14" t="inlineStr">
+        <is>
+          <t>pedro_alcantara_siveira@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D5" s="16" t="n">
+        <v>59</v>
+      </c>
+      <c r="E5" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F5" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G5" s="17" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="31.5" customHeight="1">
+      <c r="B6" s="16" t="inlineStr">
+        <is>
+          <t>cleber_cunha_dasilva@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D6" s="16" t="n">
+        <v>54</v>
+      </c>
+      <c r="E6" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F6" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G6" s="17" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="31.5" customHeight="1">
+      <c r="B7" s="16" t="inlineStr">
+        <is>
+          <t>emerencia_silveira@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D7" s="16" t="n">
+        <v>45</v>
+      </c>
+      <c r="E7" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F7" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G7" s="17" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="31.5" customHeight="1">
+      <c r="B8" s="16" t="inlineStr">
+        <is>
+          <t>ezequiel_valentim@gmail.com</t>
+        </is>
+      </c>
+      <c r="C8" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D8" s="16" t="n">
+        <v>33</v>
+      </c>
+      <c r="E8" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F8" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="31.5" customHeight="1">
+      <c r="B9" s="16" t="inlineStr">
+        <is>
+          <t>ermedovaldo_clemente@gmail.com</t>
+        </is>
+      </c>
+      <c r="C9" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D9" s="16" t="n">
+        <v>44</v>
+      </c>
+      <c r="E9" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F9" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G9" s="17" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="31.5" customHeight="1">
+      <c r="B10" s="16" t="inlineStr">
+        <is>
+          <t>jonas_pedroso@gmail.com</t>
+        </is>
+      </c>
+      <c r="C10" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D10" s="16" t="n">
+        <v>73</v>
+      </c>
+      <c r="E10" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F10" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G10" s="16" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="31.5" customHeight="1">
+      <c r="B11" s="16" t="inlineStr">
+        <is>
+          <t>nivaldo_osvaldi@gmail.com</t>
+        </is>
+      </c>
+      <c r="C11" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D11" s="16" t="n">
+        <v>32</v>
+      </c>
+      <c r="E11" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F11" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G11" s="16" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.5" customHeight="1">
+      <c r="B12" s="14" t="inlineStr">
+        <is>
+          <t>pedro_pedroso@gmail.com</t>
+        </is>
+      </c>
+      <c r="C12" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D12" s="16" t="n">
+        <v>55</v>
+      </c>
+      <c r="E12" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="F12" s="16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="G12" s="16" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="31.5" customHeight="1">
+      <c r="B13" s="16" t="inlineStr">
+        <is>
+          <t>deodoro_fonseca@gmail.com</t>
+        </is>
+      </c>
+      <c r="C13" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D13" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="E3" s="38" t="inlineStr">
+      <c r="E13" s="16" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F13" s="16" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="G13" s="16" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="31.5" customHeight="1">
+      <c r="B14" s="16" t="inlineStr">
+        <is>
+          <t>pedro_alvarez@gmail.com</t>
+        </is>
+      </c>
+      <c r="C14" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D14" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="E14" s="16" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="F14" s="16" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="G14" s="16" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="31.5" customHeight="1">
+      <c r="B15" s="16" t="inlineStr">
+        <is>
+          <t>pedro_pires_pinheiro@gmail.com</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
+        <is>
+          <t>nunsip-4kizgi-nefSyd</t>
+        </is>
+      </c>
+      <c r="D15" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" s="16" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F3" s="38" t="inlineStr">
+      <c r="F15" s="16" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G3" s="39" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="31.5" customHeight="1">
-      <c r="B4" s="38" t="inlineStr">
-        <is>
-          <t>asdrubal_dos_santos@gmail.com</t>
-        </is>
-      </c>
-      <c r="C4" s="38" t="inlineStr">
+      <c r="G15" s="16" t="inlineStr">
+        <is>
+          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="31.5" customHeight="1">
+      <c r="B16" s="16" t="inlineStr">
+        <is>
+          <t>hermedovaldo_da_silva@gmail.com</t>
+        </is>
+      </c>
+      <c r="C16" s="16" t="inlineStr">
         <is>
           <t>nunsip-4kizgi-nefSyd</t>
         </is>
       </c>
-      <c r="D4" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" s="38" t="inlineStr">
+      <c r="D16" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" s="16" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="F4" s="38" t="inlineStr">
+      <c r="F16" s="16" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="G4" s="39" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="31.5" customHeight="1">
-      <c r="B5" s="36" t="inlineStr">
-        <is>
-          <t>pedro_alcantara_siveira@gmail.com</t>
-        </is>
-      </c>
-      <c r="C5" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D5" s="38" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F5" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="G5" s="39" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="31.5" customHeight="1">
-      <c r="B6" s="38" t="inlineStr">
-        <is>
-          <t>cleber_cunha_dasilva@gmail.com</t>
-        </is>
-      </c>
-      <c r="C6" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D6" s="38" t="n">
-        <v>14</v>
-      </c>
-      <c r="E6" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F6" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="G6" s="39" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="31.5" customHeight="1">
-      <c r="B7" s="38" t="inlineStr">
-        <is>
-          <t>emerencia_silveira@gmail.com</t>
-        </is>
-      </c>
-      <c r="C7" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D7" s="38" t="n">
-        <v>15</v>
-      </c>
-      <c r="E7" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F7" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="G7" s="39" t="inlineStr">
+      <c r="G16" s="16" t="inlineStr">
         <is>
           <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="31.5" customHeight="1">
-      <c r="B8" s="38" t="inlineStr">
-        <is>
-          <t>ezequiel_valentim@gmail.com</t>
-        </is>
-      </c>
-      <c r="C8" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D8" s="38" t="n">
-        <v>13</v>
-      </c>
-      <c r="E8" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F8" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="G8" s="39" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="31.5" customHeight="1">
-      <c r="B9" s="38" t="inlineStr">
-        <is>
-          <t>ermedovaldo_clemente@gmail.com</t>
-        </is>
-      </c>
-      <c r="C9" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D9" s="38" t="n">
-        <v>14</v>
-      </c>
-      <c r="E9" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F9" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="G9" s="39" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="31.5" customHeight="1">
-      <c r="B10" s="38" t="inlineStr">
-        <is>
-          <t>jonas_pedroso@gmail.com</t>
-        </is>
-      </c>
-      <c r="C10" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D10" s="38" t="n">
-        <v>13</v>
-      </c>
-      <c r="E10" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F10" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="G10" s="38" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="31.5" customHeight="1">
-      <c r="B11" s="38" t="inlineStr">
-        <is>
-          <t>nivaldo_osvaldi@gmail.com</t>
-        </is>
-      </c>
-      <c r="C11" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D11" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F11" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="G11" s="38" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.5" customHeight="1">
-      <c r="B12" s="36" t="inlineStr">
-        <is>
-          <t>pedro_pedroso@gmail.com</t>
-        </is>
-      </c>
-      <c r="C12" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D12" s="38" t="n">
-        <v>5</v>
-      </c>
-      <c r="E12" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F12" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="G12" s="38" t="inlineStr">
-        <is>
-          <t>Conta bloqueada pelo Linkedin por muitas tentativas. Troque esta conta por outra, ou remova esta linha do Excel.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="31.5" customHeight="1">
-      <c r="B13" s="38" t="inlineStr">
-        <is>
-          <t>deodoro_fonseca@gmail.com</t>
-        </is>
-      </c>
-      <c r="C13" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D13" s="38" t="n">
-        <v>12</v>
-      </c>
-      <c r="E13" s="38" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="F13" s="38" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="G13" s="38" t="inlineStr">
-        <is>
-          <t>---</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="31.5" customHeight="1">
-      <c r="B14" s="38" t="inlineStr">
-        <is>
-          <t>pedro_alvarez@gmail.com</t>
-        </is>
-      </c>
-      <c r="C14" s="38" t="inlineStr">
-        <is>
-          <t>nunsip-4kizgi-nefSyd</t>
-        </is>
-      </c>
-      <c r="D14" s="38" t="n">
-        <v>11</v>
-      </c>
-      <c r="E14" s="38" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="F14" s="38" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="G14" s="38" t="inlineStr">
-        <is>
-          <t>Conta pede uma verificação se é um robô. Acesse o linkedin com essa conta e resolva o captcha.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15"/>
+    <row r="17"/>
   </sheetData>
   <conditionalFormatting sqref="G2 F1:F3 F13:F1048576">
     <cfRule type="cellIs" priority="8" operator="equal" dxfId="1">
@@ -3409,26 +3208,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B12" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>